<commit_message>
Add count of individuals subject to the tax. Reorganise simulation section. Update US data (tax unit level)
</commit_message>
<xml_diff>
--- a/public/wealth-tax-simulation.xlsx
+++ b/public/wealth-tax-simulation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l.mouillet\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A715135C-AF16-4046-8F3B-2A2DEC6A658D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F00C6AD-5A78-4907-96EE-AB41B3CC844B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1410" windowWidth="29040" windowHeight="15720" xr2:uid="{A69BB1AE-355D-4D40-8FE7-BE3B860A349E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A69BB1AE-355D-4D40-8FE7-BE3B860A349E}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="14" r:id="rId1"/>
@@ -25,8 +25,8 @@
     <sheet name="Balkir et al. (2025)" sheetId="10" r:id="rId10"/>
     <sheet name="Palomo et al. (2025)" sheetId="12" r:id="rId11"/>
     <sheet name="Bruil et al. (2025)" sheetId="4" r:id="rId12"/>
-    <sheet name="Billionnaires List" sheetId="19" r:id="rId13"/>
-    <sheet name="Guzzardi et al. (2024)" sheetId="16" r:id="rId14"/>
+    <sheet name="Guzzardi et al. (2024)" sheetId="16" r:id="rId13"/>
+    <sheet name="Billionnaires List" sheetId="19" r:id="rId14"/>
     <sheet name="Income to wealth ratios" sheetId="20" r:id="rId15"/>
     <sheet name="WID" sheetId="21" r:id="rId16"/>
   </sheets>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="276">
   <si>
     <t>P0-10</t>
   </si>
@@ -1116,6 +1116,15 @@
   </si>
   <si>
     <t>We use nominal income growth rates by income group and by country from the World Inequality Database.</t>
+  </si>
+  <si>
+    <t>Number of units exposed</t>
+  </si>
+  <si>
+    <t>Number of units</t>
+  </si>
+  <si>
+    <t>Household multiplier</t>
   </si>
 </sst>
 </file>
@@ -2991,9 +3000,6 @@
     <xf numFmtId="181" fontId="72" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="174" fontId="60" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3080,6 +3086,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3101,8 +3110,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="434">
@@ -3633,7 +3642,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FRA!$L$4:$L$10</c:f>
+              <c:f>FRA!$M$4:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3714,7 +3723,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FRA!$M$4:$M$10</c:f>
+              <c:f>FRA!$N$4:$N$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3987,7 +3996,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>USA!$L$4:$L$10</c:f>
+              <c:f>USA!$M$4:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4068,7 +4077,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>USA!$M$4:$M$10</c:f>
+              <c:f>USA!$N$4:$N$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4344,7 +4353,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>NDL!$L$4:$L$10</c:f>
+              <c:f>NDL!$M$4:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4425,7 +4434,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>NDL!$M$4:$M$10</c:f>
+              <c:f>NDL!$N$4:$N$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4701,7 +4710,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BRA!$L$4:$L$10</c:f>
+              <c:f>BRA!$M$4:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4784,7 +4793,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BRA!$M$4:$M$10</c:f>
+              <c:f>BRA!$N$4:$N$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5057,7 +5066,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ITA!$L$4:$L$10</c:f>
+              <c:f>ITA!$M$4:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5138,7 +5147,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ITA!$M$4:$M$10</c:f>
+              <c:f>ITA!$N$4:$N$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
@@ -8128,13 +8137,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>325426</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>37601</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>93367</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>144306</xdr:rowOff>
@@ -8169,13 +8178,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>429085</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>180778</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>196632</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>59671</xdr:rowOff>
@@ -8212,13 +8221,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>299413</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>28181</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>78849</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>37796</xdr:rowOff>
@@ -8255,13 +8264,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>339681</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>8473</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>122928</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>18088</xdr:rowOff>
@@ -8298,13 +8307,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>364592</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>27229</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>155459</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>34939</xdr:rowOff>
@@ -8636,9 +8645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2E67E3-ED89-40FD-A6A8-5FC44FD01F6F}">
   <dimension ref="A2:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
@@ -8728,7 +8735,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="125" customFormat="1">
+    <row r="26" spans="1:3" s="124" customFormat="1">
       <c r="C26" s="70" t="s">
         <v>235</v>
       </c>
@@ -8738,28 +8745,28 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="125" customFormat="1">
-      <c r="C28" s="125" t="s">
+    <row r="28" spans="1:3" s="124" customFormat="1">
+      <c r="C28" s="124" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="125" customFormat="1">
-      <c r="C29" s="125" t="s">
+    <row r="29" spans="1:3" s="124" customFormat="1">
+      <c r="C29" s="124" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="125" customFormat="1">
-      <c r="C30" s="125" t="s">
+    <row r="30" spans="1:3" s="124" customFormat="1">
+      <c r="C30" s="124" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="125" customFormat="1">
-      <c r="C31" s="125" t="s">
+    <row r="31" spans="1:3" s="124" customFormat="1">
+      <c r="C31" s="124" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="125" customFormat="1">
-      <c r="C32" s="125" t="s">
+    <row r="32" spans="1:3" s="124" customFormat="1">
+      <c r="C32" s="124" t="s">
         <v>242</v>
       </c>
     </row>
@@ -8798,8 +8805,8 @@
         <v>272</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="125" customFormat="1">
-      <c r="B42" s="125" t="s">
+    <row r="42" spans="1:3" s="124" customFormat="1">
+      <c r="B42" s="124" t="s">
         <v>270</v>
       </c>
     </row>
@@ -8853,7 +8860,7 @@
   <dimension ref="B2:J10"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -8913,7 +8920,7 @@
       <c r="D4" s="63">
         <v>452300000</v>
       </c>
-      <c r="E4" s="130">
+      <c r="E4" s="129">
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="F4" s="80">
@@ -8942,7 +8949,7 @@
       <c r="D5" s="81">
         <v>1093400000</v>
       </c>
-      <c r="E5" s="130">
+      <c r="E5" s="129">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="F5" s="30">
@@ -8971,7 +8978,7 @@
       <c r="D6" s="81">
         <v>238700000</v>
       </c>
-      <c r="E6" s="130">
+      <c r="E6" s="129">
         <v>6.3E-2</v>
       </c>
       <c r="F6" s="30">
@@ -9133,11 +9140,11 @@
       <c r="N4" s="25">
         <v>68523</v>
       </c>
-      <c r="O4" s="132">
+      <c r="O4" s="131">
         <f>M4/4.03</f>
         <v>3549.6277915632754</v>
       </c>
-      <c r="P4" s="132">
+      <c r="P4" s="131">
         <f>N4/4.03</f>
         <v>17003.225806451614</v>
       </c>
@@ -9180,11 +9187,11 @@
       <c r="N5" s="25">
         <v>141121</v>
       </c>
-      <c r="O5" s="132">
+      <c r="O5" s="131">
         <f t="shared" ref="O5:O12" si="0">M5/4.03</f>
         <v>8977.1712158808932</v>
       </c>
-      <c r="P5" s="132">
+      <c r="P5" s="131">
         <f t="shared" ref="P5:P12" si="1">N5/4.03</f>
         <v>35017.617866004963</v>
       </c>
@@ -9227,11 +9234,11 @@
       <c r="N6" s="25">
         <v>230814</v>
       </c>
-      <c r="O6" s="132">
+      <c r="O6" s="131">
         <f t="shared" si="0"/>
         <v>18166.99751861042</v>
       </c>
-      <c r="P6" s="132">
+      <c r="P6" s="131">
         <f t="shared" si="1"/>
         <v>57273.945409429274</v>
       </c>
@@ -9274,11 +9281,11 @@
       <c r="N7" s="25">
         <v>365465</v>
       </c>
-      <c r="O7" s="132">
+      <c r="O7" s="131">
         <f t="shared" si="0"/>
         <v>32040.942928039702</v>
       </c>
-      <c r="P7" s="132">
+      <c r="P7" s="131">
         <f t="shared" si="1"/>
         <v>90686.104218362278</v>
       </c>
@@ -9315,17 +9322,17 @@
       <c r="L8" s="62">
         <v>1491870</v>
       </c>
-      <c r="M8" s="134">
+      <c r="M8" s="133">
         <v>374526</v>
       </c>
-      <c r="N8" s="134">
+      <c r="N8" s="133">
         <v>1004838</v>
       </c>
-      <c r="O8" s="133">
+      <c r="O8" s="132">
         <f t="shared" si="0"/>
         <v>92934.491315136474</v>
       </c>
-      <c r="P8" s="133">
+      <c r="P8" s="132">
         <f t="shared" si="1"/>
         <v>249339.4540942928</v>
       </c>
@@ -9362,17 +9369,17 @@
       <c r="L9" s="62">
         <v>149187</v>
       </c>
-      <c r="M9" s="134">
+      <c r="M9" s="133">
         <v>1422293</v>
       </c>
-      <c r="N9" s="134">
+      <c r="N9" s="133">
         <v>4586560</v>
       </c>
-      <c r="O9" s="133">
+      <c r="O9" s="132">
         <f t="shared" si="0"/>
         <v>352926.30272952851</v>
       </c>
-      <c r="P9" s="133">
+      <c r="P9" s="132">
         <f t="shared" si="1"/>
         <v>1138104.2183622827</v>
       </c>
@@ -9409,17 +9416,17 @@
       <c r="L10" s="62">
         <v>14922</v>
       </c>
-      <c r="M10" s="134">
+      <c r="M10" s="133">
         <v>7003875</v>
       </c>
-      <c r="N10" s="134">
+      <c r="N10" s="133">
         <v>22950356</v>
       </c>
-      <c r="O10" s="133">
+      <c r="O10" s="132">
         <f t="shared" si="0"/>
         <v>1737934.2431761785</v>
       </c>
-      <c r="P10" s="133">
+      <c r="P10" s="132">
         <f t="shared" si="1"/>
         <v>5694877.4193548383</v>
       </c>
@@ -9457,17 +9464,17 @@
       <c r="L11" s="62">
         <v>1492</v>
       </c>
-      <c r="M11" s="134">
+      <c r="M11" s="133">
         <v>36343312</v>
       </c>
-      <c r="N11" s="134">
+      <c r="N11" s="133">
         <v>111879448</v>
       </c>
-      <c r="O11" s="133">
+      <c r="O11" s="132">
         <f t="shared" si="0"/>
         <v>9018191.5632754341</v>
       </c>
-      <c r="P11" s="133">
+      <c r="P11" s="132">
         <f t="shared" si="1"/>
         <v>27761649.627791561</v>
       </c>
@@ -9505,17 +9512,17 @@
       <c r="L12" s="62">
         <v>152</v>
       </c>
-      <c r="M12" s="134">
+      <c r="M12" s="133">
         <v>199694816</v>
       </c>
-      <c r="N12" s="134">
+      <c r="N12" s="133">
         <v>491618912</v>
       </c>
-      <c r="O12" s="133">
+      <c r="O12" s="132">
         <f t="shared" si="0"/>
         <v>49552063.523573197</v>
       </c>
-      <c r="P12" s="133">
+      <c r="P12" s="132">
         <f t="shared" si="1"/>
         <v>121989804.46650124</v>
       </c>
@@ -10191,243 +10198,11 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F615E9C2-9ECA-4B37-BDE5-46C3885B0ED1}">
-  <dimension ref="A1:F26"/>
-  <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="3.6640625" style="120" customWidth="1"/>
-    <col min="2" max="5" width="12.5546875" style="54" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" style="54"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:6" s="120" customFormat="1">
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-    </row>
-    <row r="2" spans="2:6" ht="28.8">
-      <c r="B2" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="C2" s="123" t="s">
-        <v>214</v>
-      </c>
-      <c r="D2" s="123" t="s">
-        <v>215</v>
-      </c>
-      <c r="E2" s="123" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6">
-      <c r="B3" s="136" t="s">
-        <v>211</v>
-      </c>
-      <c r="C3" s="128">
-        <v>147</v>
-      </c>
-      <c r="D3" s="126">
-        <v>730</v>
-      </c>
-      <c r="E3" s="127">
-        <v>695.2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4" s="136" t="s">
-        <v>217</v>
-      </c>
-      <c r="C4" s="129">
-        <v>936</v>
-      </c>
-      <c r="D4" s="126">
-        <v>7927.6093639999926</v>
-      </c>
-      <c r="E4" s="127">
-        <f>D4*0.95</f>
-        <v>7531.2288957999926</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="136" t="s">
-        <v>209</v>
-      </c>
-      <c r="C5" s="129">
-        <v>79</v>
-      </c>
-      <c r="D5" s="126">
-        <v>360.74274099999991</v>
-      </c>
-      <c r="E5" s="127">
-        <f>D5*0.95</f>
-        <v>342.7056039499999</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="32" t="s">
-        <v>210</v>
-      </c>
-      <c r="C6" s="129">
-        <v>66</v>
-      </c>
-      <c r="D6" s="126">
-        <v>252.6951380000001</v>
-      </c>
-      <c r="E6" s="127">
-        <f t="shared" ref="E6:E7" si="0">D6*0.95</f>
-        <v>240.06038110000009</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="32" t="s">
-        <v>212</v>
-      </c>
-      <c r="C7" s="129">
-        <v>13</v>
-      </c>
-      <c r="D7" s="126">
-        <v>49.210541999999997</v>
-      </c>
-      <c r="E7" s="127">
-        <f t="shared" si="0"/>
-        <v>46.750014899999996</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="121"/>
-      <c r="C8" s="122"/>
-      <c r="D8" s="122"/>
-      <c r="E8" s="122"/>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="124" t="s">
-        <v>218</v>
-      </c>
-      <c r="C9" s="122"/>
-      <c r="D9" s="122"/>
-      <c r="E9" s="122"/>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10" s="121" t="s">
-        <v>227</v>
-      </c>
-      <c r="C10" s="122"/>
-      <c r="D10" s="122"/>
-      <c r="E10" s="122"/>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11" s="121"/>
-      <c r="C11" s="122"/>
-      <c r="D11" s="122"/>
-      <c r="E11" s="122"/>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="121"/>
-      <c r="C12" s="122"/>
-      <c r="D12" s="122"/>
-      <c r="E12" s="122"/>
-    </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="121"/>
-      <c r="C13" s="122"/>
-      <c r="D13" s="122"/>
-      <c r="E13" s="122"/>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="C14" s="122"/>
-      <c r="D14" s="122"/>
-      <c r="E14" s="122"/>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="C15" s="122"/>
-      <c r="D15" s="122"/>
-      <c r="E15" s="122"/>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="B16" s="121"/>
-      <c r="C16" s="122"/>
-      <c r="D16" s="122"/>
-      <c r="E16" s="122"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="121"/>
-      <c r="C17" s="122"/>
-      <c r="D17" s="122"/>
-      <c r="E17" s="122"/>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="121"/>
-      <c r="C18" s="122"/>
-      <c r="D18" s="122"/>
-      <c r="E18" s="122"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="121"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="122"/>
-      <c r="E19" s="122"/>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="121"/>
-      <c r="C20" s="122"/>
-      <c r="D20" s="122"/>
-      <c r="E20" s="122"/>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="121"/>
-      <c r="C21" s="122"/>
-      <c r="D21" s="122"/>
-      <c r="E21" s="122"/>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="121"/>
-      <c r="C22" s="122"/>
-      <c r="D22" s="122"/>
-      <c r="E22" s="122"/>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="121"/>
-      <c r="C23" s="122"/>
-      <c r="D23" s="122"/>
-      <c r="E23" s="122"/>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="121"/>
-      <c r="C24" s="122"/>
-      <c r="D24" s="122"/>
-      <c r="E24" s="122"/>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="121"/>
-      <c r="C25" s="122"/>
-      <c r="D25" s="122"/>
-      <c r="E25" s="122"/>
-    </row>
-    <row r="26" spans="2:5">
-      <c r="B26" s="121"/>
-      <c r="C26" s="122"/>
-      <c r="D26" s="122"/>
-      <c r="E26" s="122"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2BD9FE-447D-43A9-B308-0AB122408051}">
   <dimension ref="B2:M33"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -10801,13 +10576,13 @@
       <c r="B29" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="118">
+      <c r="C29" s="117">
         <v>506994</v>
       </c>
-      <c r="D29" s="118">
+      <c r="D29" s="117">
         <v>147733</v>
       </c>
-      <c r="E29" s="118">
+      <c r="E29" s="117">
         <v>310672</v>
       </c>
       <c r="F29" s="39" t="s">
@@ -10818,13 +10593,13 @@
       <c r="B30" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="118">
+      <c r="C30" s="117">
         <v>50699</v>
       </c>
-      <c r="D30" s="118">
+      <c r="D30" s="117">
         <v>507543</v>
       </c>
-      <c r="E30" s="118">
+      <c r="E30" s="117">
         <v>1195681</v>
       </c>
       <c r="F30" s="39" t="s">
@@ -10846,6 +10621,238 @@
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="B2:D2"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F615E9C2-9ECA-4B37-BDE5-46C3885B0ED1}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" style="119" customWidth="1"/>
+    <col min="2" max="5" width="12.5546875" style="54" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" style="54"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" s="119" customFormat="1">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+    </row>
+    <row r="2" spans="2:6" ht="28.8">
+      <c r="B2" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" s="122" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2" s="122" t="s">
+        <v>215</v>
+      </c>
+      <c r="E2" s="122" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="135" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" s="127">
+        <v>147</v>
+      </c>
+      <c r="D3" s="125">
+        <v>730</v>
+      </c>
+      <c r="E3" s="126">
+        <v>695.2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="135" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="128">
+        <v>936</v>
+      </c>
+      <c r="D4" s="125">
+        <v>7927.6093639999926</v>
+      </c>
+      <c r="E4" s="126">
+        <f>D4*0.95</f>
+        <v>7531.2288957999926</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="135" t="s">
+        <v>209</v>
+      </c>
+      <c r="C5" s="128">
+        <v>79</v>
+      </c>
+      <c r="D5" s="125">
+        <v>360.74274099999991</v>
+      </c>
+      <c r="E5" s="126">
+        <f>D5*0.95</f>
+        <v>342.7056039499999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="C6" s="128">
+        <v>66</v>
+      </c>
+      <c r="D6" s="125">
+        <v>252.6951380000001</v>
+      </c>
+      <c r="E6" s="126">
+        <f t="shared" ref="E6:E7" si="0">D6*0.95</f>
+        <v>240.06038110000009</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" s="128">
+        <v>13</v>
+      </c>
+      <c r="D7" s="125">
+        <v>49.210541999999997</v>
+      </c>
+      <c r="E7" s="126">
+        <f t="shared" si="0"/>
+        <v>46.750014899999996</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="120"/>
+      <c r="C8" s="121"/>
+      <c r="D8" s="121"/>
+      <c r="E8" s="121"/>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="123" t="s">
+        <v>218</v>
+      </c>
+      <c r="C9" s="121"/>
+      <c r="D9" s="121"/>
+      <c r="E9" s="121"/>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="120" t="s">
+        <v>227</v>
+      </c>
+      <c r="C10" s="121"/>
+      <c r="D10" s="121"/>
+      <c r="E10" s="121"/>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="120"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="121"/>
+      <c r="E11" s="121"/>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="120"/>
+      <c r="C12" s="121"/>
+      <c r="D12" s="121"/>
+      <c r="E12" s="121"/>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="120"/>
+      <c r="C13" s="121"/>
+      <c r="D13" s="121"/>
+      <c r="E13" s="121"/>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="C14" s="121"/>
+      <c r="D14" s="121"/>
+      <c r="E14" s="121"/>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="C15" s="121"/>
+      <c r="D15" s="121"/>
+      <c r="E15" s="121"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="120"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="121"/>
+      <c r="E16" s="121"/>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="120"/>
+      <c r="C17" s="121"/>
+      <c r="D17" s="121"/>
+      <c r="E17" s="121"/>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="120"/>
+      <c r="C18" s="121"/>
+      <c r="D18" s="121"/>
+      <c r="E18" s="121"/>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="120"/>
+      <c r="C19" s="121"/>
+      <c r="D19" s="121"/>
+      <c r="E19" s="121"/>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="120"/>
+      <c r="C20" s="121"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="121"/>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="120"/>
+      <c r="C21" s="121"/>
+      <c r="D21" s="121"/>
+      <c r="E21" s="121"/>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="120"/>
+      <c r="C22" s="121"/>
+      <c r="D22" s="121"/>
+      <c r="E22" s="121"/>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="120"/>
+      <c r="C23" s="121"/>
+      <c r="D23" s="121"/>
+      <c r="E23" s="121"/>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="120"/>
+      <c r="C24" s="121"/>
+      <c r="D24" s="121"/>
+      <c r="E24" s="121"/>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="120"/>
+      <c r="C25" s="121"/>
+      <c r="D25" s="121"/>
+      <c r="E25" s="121"/>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="120"/>
+      <c r="C26" s="121"/>
+      <c r="D26" s="121"/>
+      <c r="E26" s="121"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -10861,20 +10868,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.21875" style="125" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" style="124" customWidth="1"/>
     <col min="4" max="4" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="28.8">
-      <c r="B2" s="131" t="s">
+      <c r="B2" s="130" t="s">
         <v>232</v>
       </c>
-      <c r="C2" s="131" t="s">
+      <c r="C2" s="130" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="3" spans="2:15">
-      <c r="B3" s="135">
+      <c r="B3" s="134">
         <v>99</v>
       </c>
       <c r="C3" s="30">
@@ -10897,7 +10904,7 @@
       <c r="O3" s="24"/>
     </row>
     <row r="4" spans="2:15">
-      <c r="B4" s="135">
+      <c r="B4" s="134">
         <v>99.099998474121094</v>
       </c>
       <c r="C4" s="30">
@@ -10917,7 +10924,7 @@
       <c r="O4" s="24"/>
     </row>
     <row r="5" spans="2:15">
-      <c r="B5" s="135">
+      <c r="B5" s="134">
         <v>99.199996948242188</v>
       </c>
       <c r="C5" s="30">
@@ -10937,7 +10944,7 @@
       <c r="O5" s="24"/>
     </row>
     <row r="6" spans="2:15">
-      <c r="B6" s="135">
+      <c r="B6" s="134">
         <v>99.300003051757813</v>
       </c>
       <c r="C6" s="30">
@@ -10957,7 +10964,7 @@
       <c r="O6" s="24"/>
     </row>
     <row r="7" spans="2:15">
-      <c r="B7" s="135">
+      <c r="B7" s="134">
         <v>99.400001525878906</v>
       </c>
       <c r="C7" s="30">
@@ -10977,7 +10984,7 @@
       <c r="O7" s="24"/>
     </row>
     <row r="8" spans="2:15">
-      <c r="B8" s="135">
+      <c r="B8" s="134">
         <v>99.5</v>
       </c>
       <c r="C8" s="30">
@@ -10997,7 +11004,7 @@
       <c r="O8" s="24"/>
     </row>
     <row r="9" spans="2:15">
-      <c r="B9" s="135">
+      <c r="B9" s="134">
         <v>99.599998474121094</v>
       </c>
       <c r="C9" s="30">
@@ -11017,7 +11024,7 @@
       <c r="O9" s="24"/>
     </row>
     <row r="10" spans="2:15">
-      <c r="B10" s="135">
+      <c r="B10" s="134">
         <v>99.699996948242188</v>
       </c>
       <c r="C10" s="30">
@@ -11037,7 +11044,7 @@
       <c r="O10" s="24"/>
     </row>
     <row r="11" spans="2:15">
-      <c r="B11" s="135">
+      <c r="B11" s="134">
         <v>99.800003051757813</v>
       </c>
       <c r="C11" s="30">
@@ -11057,7 +11064,7 @@
       <c r="O11" s="24"/>
     </row>
     <row r="12" spans="2:15">
-      <c r="B12" s="135">
+      <c r="B12" s="134">
         <v>99.900001525878906</v>
       </c>
       <c r="C12" s="30">
@@ -11077,7 +11084,7 @@
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="2:15">
-      <c r="B13" s="135">
+      <c r="B13" s="134">
         <v>99.910003662109375</v>
       </c>
       <c r="C13" s="30">
@@ -11100,7 +11107,7 @@
       <c r="O13" s="24"/>
     </row>
     <row r="14" spans="2:15">
-      <c r="B14" s="135">
+      <c r="B14" s="134">
         <v>99.919998168945313</v>
       </c>
       <c r="C14" s="30">
@@ -11120,7 +11127,7 @@
       <c r="O14" s="24"/>
     </row>
     <row r="15" spans="2:15">
-      <c r="B15" s="135">
+      <c r="B15" s="134">
         <v>99.930000305175781</v>
       </c>
       <c r="C15" s="30">
@@ -11140,7 +11147,7 @@
       <c r="O15" s="24"/>
     </row>
     <row r="16" spans="2:15">
-      <c r="B16" s="135">
+      <c r="B16" s="134">
         <v>99.94000244140625</v>
       </c>
       <c r="C16" s="30">
@@ -11160,7 +11167,7 @@
       <c r="O16" s="24"/>
     </row>
     <row r="17" spans="2:15">
-      <c r="B17" s="135">
+      <c r="B17" s="134">
         <v>99.949996948242188</v>
       </c>
       <c r="C17" s="30">
@@ -11180,7 +11187,7 @@
       <c r="O17" s="24"/>
     </row>
     <row r="18" spans="2:15">
-      <c r="B18" s="135">
+      <c r="B18" s="134">
         <v>99.959999084472656</v>
       </c>
       <c r="C18" s="30">
@@ -11200,7 +11207,7 @@
       <c r="O18" s="24"/>
     </row>
     <row r="19" spans="2:15">
-      <c r="B19" s="135">
+      <c r="B19" s="134">
         <v>99.970001220703125</v>
       </c>
       <c r="C19" s="30">
@@ -11220,7 +11227,7 @@
       <c r="O19" s="24"/>
     </row>
     <row r="20" spans="2:15">
-      <c r="B20" s="135">
+      <c r="B20" s="134">
         <v>99.980003356933594</v>
       </c>
       <c r="C20" s="30">
@@ -11240,7 +11247,7 @@
       <c r="O20" s="24"/>
     </row>
     <row r="21" spans="2:15">
-      <c r="B21" s="135">
+      <c r="B21" s="134">
         <v>99.989997863769531</v>
       </c>
       <c r="C21" s="30">
@@ -11260,7 +11267,7 @@
       <c r="O21" s="24"/>
     </row>
     <row r="22" spans="2:15">
-      <c r="B22" s="135">
+      <c r="B22" s="134">
         <v>99.990997314453125</v>
       </c>
       <c r="C22" s="30">
@@ -11283,7 +11290,7 @@
       <c r="O22" s="24"/>
     </row>
     <row r="23" spans="2:15">
-      <c r="B23" s="135">
+      <c r="B23" s="134">
         <v>99.991996765136719</v>
       </c>
       <c r="C23" s="30">
@@ -11303,7 +11310,7 @@
       <c r="O23" s="24"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="B24" s="135">
+      <c r="B24" s="134">
         <v>99.992996215820313</v>
       </c>
       <c r="C24" s="30">
@@ -11323,7 +11330,7 @@
       <c r="O24" s="24"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="B25" s="135">
+      <c r="B25" s="134">
         <v>99.994003295898438</v>
       </c>
       <c r="C25" s="30">
@@ -11343,7 +11350,7 @@
       <c r="O25" s="24"/>
     </row>
     <row r="26" spans="2:15">
-      <c r="B26" s="135">
+      <c r="B26" s="134">
         <v>99.995002746582031</v>
       </c>
       <c r="C26" s="30">
@@ -11363,7 +11370,7 @@
       <c r="O26" s="24"/>
     </row>
     <row r="27" spans="2:15">
-      <c r="B27" s="135">
+      <c r="B27" s="134">
         <v>99.996002197265625</v>
       </c>
       <c r="C27" s="30">
@@ -11383,7 +11390,7 @@
       <c r="O27" s="24"/>
     </row>
     <row r="28" spans="2:15">
-      <c r="B28" s="135">
+      <c r="B28" s="134">
         <v>99.997001647949219</v>
       </c>
       <c r="C28" s="30">
@@ -11403,7 +11410,7 @@
       <c r="O28" s="24"/>
     </row>
     <row r="29" spans="2:15">
-      <c r="B29" s="135">
+      <c r="B29" s="134">
         <v>99.998001098632813</v>
       </c>
       <c r="C29" s="30">
@@ -11423,7 +11430,7 @@
       <c r="O29" s="24"/>
     </row>
     <row r="30" spans="2:15">
-      <c r="B30" s="135">
+      <c r="B30" s="134">
         <v>99.999000549316406</v>
       </c>
       <c r="C30" s="30">
@@ -11443,7 +11450,7 @@
       <c r="O30" s="24"/>
     </row>
     <row r="31" spans="2:15">
-      <c r="B31" s="129">
+      <c r="B31" s="128">
         <v>400</v>
       </c>
       <c r="C31" s="30">
@@ -11485,7 +11492,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -11495,10 +11502,10 @@
     <col min="14" max="14" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="125" customFormat="1">
+    <row r="1" spans="1:14" s="124" customFormat="1">
       <c r="B1" s="32"/>
     </row>
-    <row r="2" spans="1:14" s="125" customFormat="1" ht="28.8">
+    <row r="2" spans="1:14" s="124" customFormat="1" ht="28.8">
       <c r="C2" s="36"/>
       <c r="D2" s="141" t="s">
         <v>267</v>
@@ -11511,12 +11518,12 @@
       <c r="J2" s="141"/>
       <c r="K2" s="141"/>
       <c r="L2" s="141"/>
-      <c r="N2" s="140" t="s">
+      <c r="N2" s="139" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="125"/>
+      <c r="A3" s="124"/>
       <c r="B3" s="56" t="s">
         <v>253</v>
       </c>
@@ -11551,7 +11558,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="125" customFormat="1">
+    <row r="4" spans="1:14" s="124" customFormat="1">
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -11568,7 +11575,7 @@
       <c r="B5" s="32" t="s">
         <v>255</v>
       </c>
-      <c r="C5" s="125" t="s">
+      <c r="C5" s="124" t="s">
         <v>256</v>
       </c>
       <c r="D5" s="81">
@@ -11608,7 +11615,7 @@
       <c r="B6" s="32" t="s">
         <v>255</v>
       </c>
-      <c r="C6" s="125" t="s">
+      <c r="C6" s="124" t="s">
         <v>257</v>
       </c>
       <c r="D6" s="81">
@@ -11648,7 +11655,7 @@
       <c r="B7" s="32" t="s">
         <v>255</v>
       </c>
-      <c r="C7" s="125" t="s">
+      <c r="C7" s="124" t="s">
         <v>258</v>
       </c>
       <c r="D7" s="81">
@@ -11688,7 +11695,7 @@
       <c r="B8" s="32" t="s">
         <v>255</v>
       </c>
-      <c r="C8" s="125" t="s">
+      <c r="C8" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D8" s="81">
@@ -11725,7 +11732,7 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="C9" s="125"/>
+      <c r="C9" s="124"/>
       <c r="D9" s="81"/>
       <c r="E9" s="81"/>
       <c r="F9" s="81"/>
@@ -11742,7 +11749,7 @@
       <c r="B10" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="125" t="s">
+      <c r="C10" s="124" t="s">
         <v>256</v>
       </c>
       <c r="D10" s="81">
@@ -11782,7 +11789,7 @@
       <c r="B11" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C11" s="125" t="s">
+      <c r="C11" s="124" t="s">
         <v>257</v>
       </c>
       <c r="D11" s="81">
@@ -11822,7 +11829,7 @@
       <c r="B12" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C12" s="125" t="s">
+      <c r="C12" s="124" t="s">
         <v>258</v>
       </c>
       <c r="D12" s="81">
@@ -11862,7 +11869,7 @@
       <c r="B13" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C13" s="125" t="s">
+      <c r="C13" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D13" s="81">
@@ -11899,7 +11906,7 @@
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="C14" s="125"/>
+      <c r="C14" s="124"/>
       <c r="D14" s="81"/>
       <c r="E14" s="81"/>
       <c r="F14" s="81"/>
@@ -11916,7 +11923,7 @@
       <c r="B15" s="32" t="s">
         <v>261</v>
       </c>
-      <c r="C15" s="125" t="s">
+      <c r="C15" s="124" t="s">
         <v>256</v>
       </c>
       <c r="D15" s="81">
@@ -11956,7 +11963,7 @@
       <c r="B16" s="32" t="s">
         <v>261</v>
       </c>
-      <c r="C16" s="125" t="s">
+      <c r="C16" s="124" t="s">
         <v>257</v>
       </c>
       <c r="D16" s="81">
@@ -11996,7 +12003,7 @@
       <c r="B17" s="32" t="s">
         <v>261</v>
       </c>
-      <c r="C17" s="125" t="s">
+      <c r="C17" s="124" t="s">
         <v>258</v>
       </c>
       <c r="D17" s="81">
@@ -12036,7 +12043,7 @@
       <c r="B18" s="32" t="s">
         <v>261</v>
       </c>
-      <c r="C18" s="125" t="s">
+      <c r="C18" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D18" s="81">
@@ -12073,7 +12080,7 @@
       </c>
     </row>
     <row r="19" spans="2:14">
-      <c r="C19" s="125"/>
+      <c r="C19" s="124"/>
       <c r="D19" s="81"/>
       <c r="E19" s="81"/>
       <c r="F19" s="81"/>
@@ -12090,7 +12097,7 @@
       <c r="B20" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="C20" s="125" t="s">
+      <c r="C20" s="124" t="s">
         <v>256</v>
       </c>
       <c r="D20" s="81">
@@ -12130,7 +12137,7 @@
       <c r="B21" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="C21" s="125" t="s">
+      <c r="C21" s="124" t="s">
         <v>257</v>
       </c>
       <c r="D21" s="81">
@@ -12170,7 +12177,7 @@
       <c r="B22" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="124" t="s">
         <v>258</v>
       </c>
       <c r="D22" s="81">
@@ -12210,7 +12217,7 @@
       <c r="B23" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="C23" s="125" t="s">
+      <c r="C23" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D23" s="81">
@@ -12247,7 +12254,7 @@
       </c>
     </row>
     <row r="24" spans="2:14">
-      <c r="C24" s="125"/>
+      <c r="C24" s="124"/>
       <c r="D24" s="81"/>
       <c r="E24" s="81"/>
       <c r="F24" s="81"/>
@@ -12264,7 +12271,7 @@
       <c r="B25" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="C25" s="125" t="s">
+      <c r="C25" s="124" t="s">
         <v>256</v>
       </c>
       <c r="D25" s="81">
@@ -12304,7 +12311,7 @@
       <c r="B26" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="C26" s="125" t="s">
+      <c r="C26" s="124" t="s">
         <v>257</v>
       </c>
       <c r="D26" s="81">
@@ -12344,7 +12351,7 @@
       <c r="B27" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="C27" s="125" t="s">
+      <c r="C27" s="124" t="s">
         <v>258</v>
       </c>
       <c r="D27" s="81">
@@ -12384,7 +12391,7 @@
       <c r="B28" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="C28" s="125" t="s">
+      <c r="C28" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D28" s="81">
@@ -12449,19 +12456,21 @@
   <sheetPr codeName="Feuil6">
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="14" width="11.5546875" customWidth="1"/>
+    <col min="2" max="11" width="11.5546875" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="124" customWidth="1"/>
+    <col min="13" max="15" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="39" customFormat="1" ht="15.6" customHeight="1">
+    <row r="1" spans="1:19" s="39" customFormat="1" ht="15.6" customHeight="1">
       <c r="A1" s="40"/>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
@@ -12476,8 +12485,9 @@
       <c r="L1" s="40"/>
       <c r="M1" s="40"/>
       <c r="N1" s="40"/>
-    </row>
-    <row r="2" spans="1:18" s="39" customFormat="1" ht="15.6" customHeight="1">
+      <c r="O1" s="40"/>
+    </row>
+    <row r="2" spans="1:19" s="39" customFormat="1" ht="15.6" customHeight="1">
       <c r="B2" s="143" t="s">
         <v>188</v>
       </c>
@@ -12497,21 +12507,22 @@
       <c r="L2" s="144"/>
       <c r="M2" s="144"/>
       <c r="N2" s="144"/>
-      <c r="O2" s="141"/>
+      <c r="O2" s="144"/>
       <c r="P2" s="141"/>
       <c r="Q2" s="141"/>
-    </row>
-    <row r="3" spans="1:18" ht="45" customHeight="1">
+      <c r="R2" s="141"/>
+    </row>
+    <row r="3" spans="1:19" ht="45" customHeight="1">
       <c r="A3" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="110" t="s">
+      <c r="B3" s="56" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" s="109" t="s">
         <v>197</v>
       </c>
-      <c r="D3" s="110" t="s">
+      <c r="D3" s="109" t="s">
         <v>192</v>
       </c>
       <c r="E3" s="53" t="s">
@@ -12520,10 +12531,10 @@
       <c r="F3" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="107" t="s">
+      <c r="G3" s="106" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="108" t="s">
+      <c r="H3" s="107" t="s">
         <v>179</v>
       </c>
       <c r="I3" s="56" t="s">
@@ -12535,21 +12546,24 @@
       <c r="K3" s="50" t="s">
         <v>196</v>
       </c>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="50" t="s">
+        <v>273</v>
+      </c>
+      <c r="M3" s="56" t="s">
         <v>181</v>
       </c>
-      <c r="M3" s="50" t="s">
+      <c r="N3" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="N3" s="56" t="s">
+      <c r="O3" s="56" t="s">
         <v>134</v>
       </c>
-      <c r="O3" s="53"/>
       <c r="P3" s="53"/>
       <c r="Q3" s="53"/>
-      <c r="R3" s="55"/>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="R3" s="53"/>
+      <c r="S3" s="55"/>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="49" t="s">
         <v>66</v>
       </c>
@@ -12560,23 +12574,24 @@
         <v>0.29750000000000004</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="108"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="84">
-        <f t="shared" ref="L4:L10" si="0">E4</f>
+      <c r="L4" s="7"/>
+      <c r="M4" s="84">
+        <f t="shared" ref="M4:M10" si="0">E4</f>
         <v>0.29750000000000004</v>
       </c>
-      <c r="M4" s="85">
-        <f>L4</f>
+      <c r="N4" s="85">
+        <f>M4</f>
         <v>0.29750000000000004</v>
       </c>
-      <c r="O4" s="48"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="45"/>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="P4" s="48"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="45"/>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="49" t="s">
         <v>67</v>
       </c>
@@ -12587,23 +12602,24 @@
         <v>0.39249999999999996</v>
       </c>
       <c r="F5" s="13"/>
-      <c r="G5" s="109"/>
-      <c r="H5" s="109"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="108"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
-      <c r="L5" s="84">
+      <c r="L5" s="7"/>
+      <c r="M5" s="84">
         <f t="shared" si="0"/>
         <v>0.39249999999999996</v>
       </c>
-      <c r="M5" s="85">
-        <f>L5</f>
+      <c r="N5" s="85">
+        <f>M5</f>
         <v>0.39249999999999996</v>
       </c>
-      <c r="O5" s="48"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="45"/>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="P5" s="48"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="45"/>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="49" t="s">
         <v>37</v>
       </c>
@@ -12614,23 +12630,24 @@
         <v>0.46499999999999997</v>
       </c>
       <c r="F6" s="13"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="84">
+      <c r="L6" s="7"/>
+      <c r="M6" s="84">
         <f t="shared" si="0"/>
         <v>0.46499999999999997</v>
       </c>
-      <c r="M6" s="85">
-        <f>L6</f>
+      <c r="N6" s="85">
+        <f>M6</f>
         <v>0.46499999999999997</v>
       </c>
-      <c r="O6" s="48"/>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="45"/>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="P6" s="48"/>
+      <c r="Q6" s="51"/>
+      <c r="R6" s="45"/>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="49" t="s">
         <v>38</v>
       </c>
@@ -12646,7 +12663,7 @@
         <f>'Bach et al. (2025)'!O15</f>
         <v>180000</v>
       </c>
-      <c r="E7" s="103">
+      <c r="E7" s="102">
         <f xml:space="preserve"> AVERAGE('Bach et al. (2025)'!J14:J22) / 100 + AVERAGE('Bozio et al. (2020)'!D14:D15)</f>
         <v>0.49282222222222216</v>
       </c>
@@ -12654,14 +12671,14 @@
         <f>(AVERAGE('Bach et al. (2025)'!C14:C22)+AVERAGE('Bach et al. (2025)'!D14:D22))/100</f>
         <v>0.15954444444444449</v>
       </c>
-      <c r="G7" s="109">
+      <c r="G7" s="108">
         <v>0.13</v>
       </c>
-      <c r="H7" s="148">
+      <c r="H7" s="140">
         <f>WID!N13</f>
         <v>3.4485277763562694E-2</v>
       </c>
-      <c r="I7" s="105">
+      <c r="I7" s="104">
         <f>(D7/G7)*(1+H7)^9/1000000</f>
         <v>1.8786591081741626</v>
       </c>
@@ -12673,23 +12690,27 @@
         <f>IF(J$13&lt;=I7, 1, (I7/J$13)^(1/(J7-1)))</f>
         <v>7.5096035696152366E-4</v>
       </c>
-      <c r="L7" s="84">
+      <c r="L7" s="63">
+        <f>IF(J$13&lt;=I7, 1, (I7/J$13)^(J7/(J7-1)))*B7</f>
+        <v>4.8037689418162675</v>
+      </c>
+      <c r="M7" s="84">
         <f t="shared" si="0"/>
         <v>0.49282222222222216</v>
       </c>
-      <c r="M7" s="85">
+      <c r="N7" s="85">
         <f>E7+MAX(0,J$14/G7-F7)*K7</f>
         <v>0.49282222222222216</v>
       </c>
-      <c r="N7" s="65">
-        <f>(M7-L7)*C7*B7*(1+H7)^9/1000000</f>
+      <c r="O7" s="65">
+        <f>(N7-M7)*C7*B7*(1+H7)^9/1000000</f>
         <v>0</v>
       </c>
-      <c r="O7" s="48"/>
-      <c r="P7" s="51"/>
-      <c r="Q7" s="45"/>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="P7" s="48"/>
+      <c r="Q7" s="51"/>
+      <c r="R7" s="45"/>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="49" t="s">
         <v>39</v>
       </c>
@@ -12705,7 +12726,7 @@
         <f>'Bach et al. (2025)'!O16</f>
         <v>626000</v>
       </c>
-      <c r="E8" s="103">
+      <c r="E8" s="102">
         <f xml:space="preserve"> AVERAGE('Bach et al. (2025)'!J23:J31) / 100 + 'Bozio et al. (2020)'!D16</f>
         <v>0.51741111111111104</v>
       </c>
@@ -12713,14 +12734,14 @@
         <f>(AVERAGE('Bach et al. (2025)'!C23:C31)+AVERAGE('Bach et al. (2025)'!D23:D31))/100</f>
         <v>0.1647777777777778</v>
       </c>
-      <c r="G8" s="109">
+      <c r="G8" s="108">
         <v>0.12</v>
       </c>
-      <c r="H8" s="148">
+      <c r="H8" s="140">
         <f>WID!N12</f>
         <v>5.4291187882988368E-2</v>
       </c>
-      <c r="I8" s="105">
+      <c r="I8" s="104">
         <f>(D8/G8)*(1+H8)^9/1000000</f>
         <v>8.3953397484216481</v>
       </c>
@@ -12732,23 +12753,27 @@
         <f>IF(J$13&lt;=I8, 1, (I8/J$13)^(1/(J8-1)))</f>
         <v>2.6429768742807939E-2</v>
       </c>
-      <c r="L8" s="84">
+      <c r="L8" s="63">
+        <f t="shared" ref="L8:L10" si="1">IF(J$13&lt;=I8, 1, (I8/J$13)^(J8/(J8-1)))*B8</f>
+        <v>75.552485387183808</v>
+      </c>
+      <c r="M8" s="84">
         <f t="shared" si="0"/>
         <v>0.51741111111111104</v>
       </c>
-      <c r="M8" s="85">
+      <c r="N8" s="85">
         <f>E8+MAX(0,J$14/G8-F8)*K8</f>
         <v>0.51746103400762522</v>
       </c>
-      <c r="N8" s="65">
-        <f>(M8-L8)*C8*B8*(1+H8)^9/1000000</f>
+      <c r="O8" s="65">
+        <f>(N8-M8)*C8*B8*(1+H8)^9/1000000</f>
         <v>2.8802785323826221</v>
       </c>
-      <c r="O8" s="48"/>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="45"/>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="P8" s="48"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="45"/>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="49" t="s">
         <v>84</v>
       </c>
@@ -12772,14 +12797,14 @@
         <f xml:space="preserve"> (AVERAGE('Bach et al. (2025)'!C32:C40, AVERAGE('Bach et al. (2025)'!C41:C44)) + AVERAGE('Bach et al. (2025)'!D32:D40, AVERAGE('Bach et al. (2025)'!D41:D44)))/100</f>
         <v>0.10618500000000002</v>
       </c>
-      <c r="G9" s="109">
+      <c r="G9" s="108">
         <v>0.09</v>
       </c>
-      <c r="H9" s="148">
+      <c r="H9" s="140">
         <f>AVERAGE(WID!N10:N11)</f>
         <v>9.585831077982554E-2</v>
       </c>
-      <c r="I9" s="105">
+      <c r="I9" s="104">
         <f>(D9/G9)*(1+H9)^9/1000000</f>
         <v>65.642050367508105</v>
       </c>
@@ -12791,23 +12816,27 @@
         <f>IF(J$13&lt;=I9, 1, (I9/J$13)^(1/(J9-1)))</f>
         <v>0.76673869192104982</v>
       </c>
-      <c r="L9" s="84">
+      <c r="L9" s="63">
+        <f t="shared" si="1"/>
+        <v>1866.2475178372611</v>
+      </c>
+      <c r="M9" s="84">
         <f t="shared" si="0"/>
         <v>0.46242699999999998</v>
       </c>
-      <c r="M9" s="85">
+      <c r="N9" s="85">
         <f>E9+MAX(0,J$14/G9-F9)*K9</f>
         <v>0.5513972279808188</v>
       </c>
-      <c r="N9" s="65">
-        <f>(M9-L9)*C9*B9*(1+H9)^9/1000000</f>
+      <c r="O9" s="65">
+        <f>(N9-M9)*C9*B9*(1+H9)^9/1000000</f>
         <v>5037.8619165823056</v>
       </c>
-      <c r="O9" s="48"/>
-      <c r="P9" s="51"/>
-      <c r="Q9" s="45"/>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="P9" s="48"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="45"/>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="49" t="s">
         <v>69</v>
       </c>
@@ -12815,7 +12844,7 @@
         <f>'Bach et al. (2025)'!N19</f>
         <v>75</v>
       </c>
-      <c r="C10" s="104">
+      <c r="C10" s="103">
         <f>'Bach et al. (2025)'!P19</f>
         <v>217289000</v>
       </c>
@@ -12831,14 +12860,14 @@
         <f xml:space="preserve"> 'Bach et al. (2025)'!C45 / 100 + 'Bach et al. (2025)'!D45 / 100</f>
         <v>1.3499999999999998E-2</v>
       </c>
-      <c r="G10" s="137">
+      <c r="G10" s="136">
         <v>0.06</v>
       </c>
-      <c r="H10" s="148">
+      <c r="H10" s="140">
         <f>WID!N10</f>
         <v>0.11952495337432567</v>
       </c>
-      <c r="I10" s="106">
+      <c r="I10" s="105">
         <f>(D10/G10)*(1+H10)^9/1000000</f>
         <v>2833.4153647951871</v>
       </c>
@@ -12850,38 +12879,46 @@
         <f>IF(J$13&lt;=I10, 1, (I10/J$13)^(1/(J10-1)))</f>
         <v>1</v>
       </c>
-      <c r="L10" s="84">
+      <c r="L10" s="63">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="M10" s="84">
         <f t="shared" si="0"/>
         <v>0.26035999999999998</v>
       </c>
-      <c r="M10" s="85">
+      <c r="N10" s="85">
         <f>E10+MAX(0,J$14/G10-F10)*K10</f>
         <v>0.58019333333333334</v>
       </c>
-      <c r="N10" s="65">
-        <f>(M10-L10)*C10*B10*(1+H10)^9/1000000</f>
+      <c r="O10" s="65">
+        <f>(N10-M10)*C10*B10*(1+H10)^9/1000000</f>
         <v>14398.814345726558</v>
       </c>
-      <c r="O10" s="48"/>
-      <c r="P10" s="51"/>
-      <c r="Q10" s="45"/>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="P10" s="48"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="45"/>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="49"/>
       <c r="F11" s="45"/>
-      <c r="G11" s="138">
+      <c r="G11" s="137">
         <f>C10*(1+H10)^9/('Billionnaires List'!E3*1000000000/'Billionnaires List'!C3)</f>
         <v>0.12692562646935071</v>
       </c>
-      <c r="N11" s="65">
-        <f>SUM(N7:N10)</f>
+      <c r="L11" s="63">
+        <f>SUM(L7:L10)</f>
+        <v>2021.603772166261</v>
+      </c>
+      <c r="O11" s="100">
+        <f>SUM(O7:O10)</f>
         <v>19439.556540841244</v>
       </c>
-      <c r="O11" s="48"/>
-      <c r="P11" s="51"/>
-      <c r="Q11" s="45"/>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="P11" s="48"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="45"/>
+    </row>
+    <row r="12" spans="1:19">
       <c r="B12" s="8" t="s">
         <v>128</v>
       </c>
@@ -12889,19 +12926,19 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="139" t="s">
+      <c r="G12" s="138" t="s">
         <v>228</v>
       </c>
       <c r="I12" s="145" t="s">
         <v>77</v>
       </c>
       <c r="J12" s="145"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="51"/>
-      <c r="Q12" s="44"/>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="O12" s="57"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="51"/>
+      <c r="R12" s="44"/>
+    </row>
+    <row r="13" spans="1:19">
       <c r="B13" t="s">
         <v>195</v>
       </c>
@@ -12912,11 +12949,11 @@
       <c r="J13" s="5">
         <v>100</v>
       </c>
-      <c r="O13" s="48"/>
-      <c r="P13" s="51"/>
-      <c r="Q13" s="44"/>
-    </row>
-    <row r="14" spans="1:18">
+      <c r="P13" s="48"/>
+      <c r="Q13" s="51"/>
+      <c r="R13" s="44"/>
+    </row>
+    <row r="14" spans="1:19">
       <c r="F14" s="45"/>
       <c r="I14" s="49" t="s">
         <v>74</v>
@@ -12924,49 +12961,49 @@
       <c r="J14" s="14">
         <v>0.02</v>
       </c>
-      <c r="O14" s="48"/>
-      <c r="P14" s="51"/>
-      <c r="Q14" s="44"/>
-    </row>
-    <row r="15" spans="1:18">
+      <c r="P14" s="48"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="44"/>
+    </row>
+    <row r="15" spans="1:19">
       <c r="C15" s="42"/>
       <c r="D15" s="42"/>
       <c r="E15" s="42"/>
       <c r="F15" s="45"/>
-      <c r="O15" s="48"/>
-      <c r="P15" s="51"/>
-      <c r="Q15" s="44"/>
-    </row>
-    <row r="16" spans="1:18">
+      <c r="P15" s="48"/>
+      <c r="Q15" s="51"/>
+      <c r="R15" s="44"/>
+    </row>
+    <row r="16" spans="1:19">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="15"/>
       <c r="F16" s="43"/>
-      <c r="O16" s="51"/>
       <c r="P16" s="51"/>
-      <c r="Q16" s="44"/>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="Q16" s="51"/>
+      <c r="R16" s="44"/>
+    </row>
+    <row r="17" spans="1:18">
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="43"/>
-      <c r="O17" s="51"/>
       <c r="P17" s="51"/>
-      <c r="Q17" s="44"/>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="Q17" s="51"/>
+      <c r="R17" s="44"/>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="47"/>
       <c r="B18" s="46"/>
       <c r="C18" s="46"/>
       <c r="D18" s="46"/>
       <c r="E18" s="46"/>
       <c r="F18" s="43"/>
-      <c r="O18" s="51"/>
       <c r="P18" s="51"/>
-      <c r="Q18" s="44"/>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="Q18" s="51"/>
+      <c r="R18" s="44"/>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="54"/>
       <c r="B19" s="54"/>
       <c r="C19" s="54"/>
@@ -12981,11 +13018,12 @@
       <c r="L19" s="54"/>
       <c r="M19" s="54"/>
       <c r="N19" s="54"/>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="C20" s="119"/>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="O19" s="54"/>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="C20" s="118"/>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="52"/>
       <c r="B22" s="54"/>
       <c r="C22" s="54"/>
@@ -13000,8 +13038,9 @@
       <c r="L22" s="54"/>
       <c r="M22" s="54"/>
       <c r="N22" s="54"/>
-    </row>
-    <row r="23" spans="1:17">
+      <c r="O22" s="54"/>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" s="54"/>
       <c r="B23" s="54"/>
       <c r="C23" s="54"/>
@@ -13016,17 +13055,18 @@
       <c r="L23" s="54"/>
       <c r="M23" s="54"/>
       <c r="N23" s="54"/>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="O23" s="54"/>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" s="54"/>
       <c r="B24" s="54"/>
       <c r="C24" s="54"/>
       <c r="D24" s="54"/>
       <c r="E24" s="54"/>
       <c r="F24" s="54"/>
-      <c r="N24" s="54"/>
-    </row>
-    <row r="25" spans="1:17">
+      <c r="O24" s="54"/>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="54"/>
       <c r="B25" s="54"/>
       <c r="C25" s="54"/>
@@ -13040,9 +13080,10 @@
       <c r="K25" s="58"/>
       <c r="L25" s="58"/>
       <c r="M25" s="58"/>
-      <c r="N25" s="54"/>
-    </row>
-    <row r="26" spans="1:17">
+      <c r="N25" s="58"/>
+      <c r="O25" s="54"/>
+    </row>
+    <row r="26" spans="1:18">
       <c r="G26" s="54"/>
       <c r="H26" s="54"/>
       <c r="I26" s="54"/>
@@ -13050,13 +13091,14 @@
       <c r="K26" s="54"/>
       <c r="L26" s="54"/>
       <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="P2:R2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="I2:O2"/>
     <mergeCell ref="I12:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13073,18 +13115,19 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A2:N16"/>
+  <dimension ref="A2:O18"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="6" width="11.5546875" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="124"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" s="39"/>
       <c r="B2" s="143" t="s">
         <v>187</v>
@@ -13105,18 +13148,19 @@
       <c r="L2" s="144"/>
       <c r="M2" s="144"/>
       <c r="N2" s="144"/>
-    </row>
-    <row r="3" spans="1:14" ht="48">
+      <c r="O2" s="144"/>
+    </row>
+    <row r="3" spans="1:15" ht="48">
       <c r="A3" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="110" t="s">
+      <c r="B3" s="56" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="D3" s="110" t="s">
+      <c r="D3" s="109" t="s">
         <v>224</v>
       </c>
       <c r="E3" s="53" t="s">
@@ -13140,17 +13184,20 @@
       <c r="K3" s="50" t="s">
         <v>196</v>
       </c>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="50" t="s">
+        <v>273</v>
+      </c>
+      <c r="M3" s="56" t="s">
         <v>181</v>
       </c>
-      <c r="M3" s="50" t="s">
+      <c r="N3" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="N3" s="56" t="s">
+      <c r="O3" s="56" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="49" t="s">
         <v>66</v>
       </c>
@@ -13165,16 +13212,17 @@
       <c r="H4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="75">
-        <f t="shared" ref="L4:L10" si="0">E4</f>
+      <c r="L4" s="7"/>
+      <c r="M4" s="75">
+        <f>E4</f>
         <v>0.24399999999999999</v>
       </c>
-      <c r="M4" s="77">
-        <f>L4</f>
+      <c r="N4" s="77">
+        <f>M4</f>
         <v>0.24399999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" s="49" t="s">
         <v>67</v>
       </c>
@@ -13189,16 +13237,17 @@
       <c r="H5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
-      <c r="L5" s="75">
-        <f t="shared" si="0"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="75">
+        <f>E5</f>
         <v>0.27224999999999999</v>
       </c>
-      <c r="M5" s="77">
-        <f>L5</f>
+      <c r="N5" s="77">
+        <f>M5</f>
         <v>0.27224999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" s="49" t="s">
         <v>37</v>
       </c>
@@ -13213,30 +13262,31 @@
       <c r="H6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="75">
-        <f t="shared" si="0"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="75">
+        <f>E6</f>
         <v>0.28149999999999997</v>
       </c>
-      <c r="M6" s="77">
-        <f>L6</f>
+      <c r="N6" s="77">
+        <f>M6</f>
         <v>0.28149999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" s="49" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="24">
-        <f>'Saez &amp; Zucman (2019)'!C15</f>
-        <v>1950271</v>
+        <f>'Saez &amp; Zucman (2019)'!C15/B18</f>
+        <v>1083483.8888888888</v>
       </c>
       <c r="C7" s="81">
-        <f>'Saez &amp; Zucman (2019)'!D15</f>
-        <v>936385</v>
+        <f>'Saez &amp; Zucman (2019)'!D15*B18</f>
+        <v>1685493</v>
       </c>
       <c r="D7" s="81">
-        <f>'Saez &amp; Zucman (2019)'!E15</f>
-        <v>539000</v>
+        <f>'Saez &amp; Zucman (2019)'!E15*B18</f>
+        <v>970200</v>
       </c>
       <c r="E7" s="30">
         <f>'Saez &amp; Zucman (2019)'!F15</f>
@@ -13246,16 +13296,16 @@
         <f>SUM('Saez &amp; Zucman (2019)'!H15,'Saez &amp; Zucman (2019)'!J15)</f>
         <v>0.19700000000000001</v>
       </c>
-      <c r="G7" s="109">
+      <c r="G7" s="108">
         <v>0.13</v>
       </c>
       <c r="H7" s="30">
         <f>WID!N28</f>
         <v>3.9354671637484406E-2</v>
       </c>
-      <c r="I7" s="105">
+      <c r="I7" s="104">
         <f>(D7/G7)*(1+H7)^9/1000000</f>
-        <v>5.8683953570913872</v>
+        <v>10.563111642764495</v>
       </c>
       <c r="J7" s="95">
         <f>C7/D7</f>
@@ -13263,36 +13313,40 @@
       </c>
       <c r="K7" s="95">
         <f>IF(J$13&lt;=I7, 1, (I7/J$13)^(1/(J7-1)))</f>
-        <v>2.1362889609356128E-2</v>
-      </c>
-      <c r="L7" s="75">
-        <f t="shared" si="0"/>
+        <v>4.7413636114533919E-2</v>
+      </c>
+      <c r="L7" s="63">
+        <f>IF(J$13&lt;=I7, 1, (I7/J$13)^(J7/(J7-1)))*B7</f>
+        <v>5426.472295445471</v>
+      </c>
+      <c r="M7" s="75">
+        <f>E7</f>
         <v>0.28899999999999998</v>
       </c>
-      <c r="M7" s="77">
+      <c r="N7" s="77">
         <f>E7+MAX(0,J$14/G7-F7)*K7</f>
         <v>0.28899999999999998</v>
       </c>
-      <c r="N7" s="65">
-        <f>(M7-L7)*C7*B7*(1+H7)^9/1000000</f>
+      <c r="O7" s="65">
+        <f>(N7-M7)*C7*B7*(1+H7)^9/1000000</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" s="49" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="24">
-        <f>'Saez &amp; Zucman (2019)'!C16</f>
-        <v>195016</v>
+        <f>'Saez &amp; Zucman (2019)'!C16/B18</f>
+        <v>108342.22222222222</v>
       </c>
       <c r="C8" s="81">
-        <f>'Saez &amp; Zucman (2019)'!D16</f>
-        <v>4526004</v>
+        <f>'Saez &amp; Zucman (2019)'!D16*B18</f>
+        <v>8146807.2000000002</v>
       </c>
       <c r="D8" s="81">
-        <f>'Saez &amp; Zucman (2019)'!E16</f>
-        <v>2430000</v>
+        <f>'Saez &amp; Zucman (2019)'!E16*B18</f>
+        <v>4374000</v>
       </c>
       <c r="E8" s="30">
         <f>'Saez &amp; Zucman (2019)'!F16</f>
@@ -13302,16 +13356,16 @@
         <f>SUM('Saez &amp; Zucman (2019)'!H16,'Saez &amp; Zucman (2019)'!J16)</f>
         <v>0.22600000000000001</v>
       </c>
-      <c r="G8" s="109">
+      <c r="G8" s="108">
         <v>0.12</v>
       </c>
       <c r="H8" s="30">
         <f>WID!N27</f>
         <v>4.5765327216810592E-2</v>
       </c>
-      <c r="I8" s="105">
+      <c r="I8" s="104">
         <f>(D8/G8)*(1+H8)^9/1000000</f>
-        <v>30.292364519812669</v>
+        <v>54.526256135662805</v>
       </c>
       <c r="J8" s="95">
         <f>C8/D8</f>
@@ -13319,36 +13373,40 @@
       </c>
       <c r="K8" s="95">
         <f>IF(J$13&lt;=I8, 1, (I8/J$13)^(1/(J8-1)))</f>
-        <v>0.25042874044366842</v>
-      </c>
-      <c r="L8" s="75">
-        <f t="shared" si="0"/>
+        <v>0.49503291399867161</v>
+      </c>
+      <c r="L8" s="63">
+        <f t="shared" ref="L8:L10" si="0">IF(J$13&lt;=I8, 1, (I8/J$13)^(J8/(J8-1)))*B8</f>
+        <v>29244.048401094864</v>
+      </c>
+      <c r="M8" s="75">
+        <f>E8</f>
         <v>0.33100000000000002</v>
       </c>
-      <c r="M8" s="77">
+      <c r="N8" s="77">
         <f>E8+MAX(0,J$14/G8-F8)*K8</f>
         <v>0.33100000000000002</v>
       </c>
-      <c r="N8" s="65">
-        <f>(M8-L8)*C8*B8*(1+H8)^9/1000000</f>
+      <c r="O8" s="65">
+        <f>(N8-M8)*C8*B8*(1+H8)^9/1000000</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" s="49" t="s">
         <v>84</v>
       </c>
       <c r="B9" s="24">
-        <f>'Saez &amp; Zucman (2019)'!C17</f>
-        <v>21163</v>
+        <f>'Saez &amp; Zucman (2019)'!C17/B18</f>
+        <v>11757.222222222223</v>
       </c>
       <c r="C9" s="81">
-        <f>'Saez &amp; Zucman (2019)'!D17</f>
-        <v>31593939</v>
+        <f>'Saez &amp; Zucman (2019)'!D17*B18</f>
+        <v>56869090.200000003</v>
       </c>
       <c r="D9" s="81">
-        <f>'Saez &amp; Zucman (2019)'!E17</f>
-        <v>12800000</v>
+        <f>'Saez &amp; Zucman (2019)'!E17*B18</f>
+        <v>23040000</v>
       </c>
       <c r="E9" s="30">
         <f>'Saez &amp; Zucman (2019)'!F17</f>
@@ -13358,16 +13416,16 @@
         <f>SUM('Saez &amp; Zucman (2019)'!H17,'Saez &amp; Zucman (2019)'!J17)</f>
         <v>0.187</v>
       </c>
-      <c r="G9" s="109">
+      <c r="G9" s="108">
         <v>0.09</v>
       </c>
       <c r="H9" s="30">
         <f>AVERAGE(WID!N25:N26)</f>
         <v>5.8166908113852278E-2</v>
       </c>
-      <c r="I9" s="105">
+      <c r="I9" s="104">
         <f>(D9/G9)*(1+H9)^9/1000000</f>
-        <v>236.56747925841836</v>
+        <v>425.82146266515298</v>
       </c>
       <c r="J9" s="95">
         <f>C9/D9</f>
@@ -13377,20 +13435,24 @@
         <f>IF(J$13&lt;=I9, 1, (I9/J$13)^(1/(J9-1)))</f>
         <v>1</v>
       </c>
-      <c r="L9" s="75">
+      <c r="L9" s="63">
         <f t="shared" si="0"/>
+        <v>11757.222222222223</v>
+      </c>
+      <c r="M9" s="75">
+        <f>E9</f>
         <v>0.30399999999999999</v>
       </c>
-      <c r="M9" s="77">
+      <c r="N9" s="77">
         <f>E9+MAX(0,J$14/G9-F9)*K9</f>
         <v>0.3392222222222222</v>
       </c>
-      <c r="N9" s="65">
-        <f>(M9-L9)*C9*B9*(1+H9)^9/1000000</f>
-        <v>39172.865561694947</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="O9" s="65">
+        <f>(N9-M9)*C9*B9*(1+H9)^9/1000000</f>
+        <v>39172.865561694955</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="49" t="s">
         <v>69</v>
       </c>
@@ -13398,11 +13460,11 @@
         <f>'Balkir et al. (2025)'!C4</f>
         <v>367</v>
       </c>
-      <c r="C10" s="112">
+      <c r="C10" s="111">
         <f>'Balkir et al. (2025)'!D4</f>
         <v>452300000</v>
       </c>
-      <c r="D10" s="112">
+      <c r="D10" s="111">
         <f>C10/3.44</f>
         <v>131482558.13953489</v>
       </c>
@@ -13414,14 +13476,14 @@
         <f>SUM('Saez &amp; Zucman (2019)'!H18,'Saez &amp; Zucman (2019)'!J18)*('Balkir et al. (2025)'!F4/'Saez &amp; Zucman (2019)'!F18)</f>
         <v>9.6234782608695627E-2</v>
       </c>
-      <c r="G10" s="137">
+      <c r="G10" s="136">
         <v>0.06</v>
       </c>
       <c r="H10" s="30">
         <f>WID!N25</f>
         <v>6.386551221830894E-2</v>
       </c>
-      <c r="I10" s="106">
+      <c r="I10" s="105">
         <f>(D10/G10)*(1+H10)^9/1000000</f>
         <v>3825.5815870854422</v>
       </c>
@@ -13433,32 +13495,40 @@
         <f>IF(J$13&lt;=I10, 1, (I10/J$13)^(1/(J10-1)))</f>
         <v>1</v>
       </c>
-      <c r="L10" s="75">
+      <c r="L10" s="63">
         <f t="shared" si="0"/>
+        <v>367</v>
+      </c>
+      <c r="M10" s="75">
+        <f t="shared" ref="M10" si="1">E10</f>
         <v>0.23799999999999999</v>
       </c>
-      <c r="M10" s="77">
+      <c r="N10" s="77">
         <f>E10+MAX(0,J$14/G10-F10)*K10</f>
         <v>0.47509855072463775</v>
       </c>
-      <c r="N10" s="65">
-        <f>(M10-L10)*C10*B10*(1+H10)^9/1000000</f>
+      <c r="O10" s="65">
+        <f>(N10-M10)*C10*B10*(1+H10)^9/1000000</f>
         <v>68707.180187923979</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" s="49"/>
       <c r="F11" s="45"/>
-      <c r="G11" s="138">
+      <c r="G11" s="137">
         <f>C10*(1+H10)^9/('Billionnaires List'!D4*1000000000/'Billionnaires List'!C4)</f>
         <v>9.3226798030417196E-2</v>
       </c>
-      <c r="N11" s="65">
-        <f>SUM(N7:N10)</f>
+      <c r="L11" s="63">
+        <f>SUM(L7:L10)</f>
+        <v>46794.742918762553</v>
+      </c>
+      <c r="O11" s="65">
+        <f>SUM(O7:O10)</f>
         <v>107880.04574961893</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="B12" s="8" t="s">
         <v>127</v>
       </c>
@@ -13466,7 +13536,7 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="139" t="s">
+      <c r="G12" s="138" t="s">
         <v>229</v>
       </c>
       <c r="I12" s="145" t="s">
@@ -13474,7 +13544,7 @@
       </c>
       <c r="J12" s="145"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="B13" t="s">
         <v>201</v>
       </c>
@@ -13486,7 +13556,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="B14" t="s">
         <v>202</v>
       </c>
@@ -13501,7 +13571,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="B15" t="s">
         <v>203</v>
       </c>
@@ -13510,15 +13580,25 @@
       <c r="E15" s="5"/>
       <c r="F15" s="45"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="43"/>
     </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18">
+        <v>1.8</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="I2:O2"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="G2:H2"/>
@@ -13536,18 +13616,19 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A2:N16"/>
+  <dimension ref="A2:O16"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="5" width="11.5546875" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="124"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" s="39"/>
       <c r="B2" s="143" t="s">
         <v>186</v>
@@ -13568,18 +13649,19 @@
       <c r="L2" s="144"/>
       <c r="M2" s="144"/>
       <c r="N2" s="144"/>
-    </row>
-    <row r="3" spans="1:14" ht="48">
+      <c r="O2" s="144"/>
+    </row>
+    <row r="3" spans="1:15" ht="48">
       <c r="A3" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="110" t="s">
+      <c r="B3" s="56" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="D3" s="110" t="s">
+      <c r="D3" s="109" t="s">
         <v>224</v>
       </c>
       <c r="E3" s="53" t="s">
@@ -13603,17 +13685,20 @@
       <c r="K3" s="50" t="s">
         <v>196</v>
       </c>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="148" t="s">
+        <v>273</v>
+      </c>
+      <c r="M3" s="56" t="s">
         <v>181</v>
       </c>
-      <c r="M3" s="50" t="s">
+      <c r="N3" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="N3" s="56" t="s">
+      <c r="O3" s="56" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="49" t="s">
         <v>66</v>
       </c>
@@ -13629,16 +13714,17 @@
       <c r="I4" s="32"/>
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
-      <c r="L4" s="74">
-        <f t="shared" ref="L4:L10" si="0">E4</f>
+      <c r="L4" s="81"/>
+      <c r="M4" s="74">
+        <f t="shared" ref="M4:M10" si="0">E4</f>
         <v>0.47125</v>
       </c>
-      <c r="M4" s="76">
-        <f>L4</f>
+      <c r="N4" s="76">
+        <f>M4</f>
         <v>0.47125</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" s="49" t="s">
         <v>67</v>
       </c>
@@ -13654,16 +13740,17 @@
       <c r="I5" s="32"/>
       <c r="J5" s="32"/>
       <c r="K5" s="32"/>
-      <c r="L5" s="74">
+      <c r="L5" s="81"/>
+      <c r="M5" s="74">
         <f t="shared" si="0"/>
         <v>0.47249999999999998</v>
       </c>
-      <c r="M5" s="76">
-        <f>L5</f>
+      <c r="N5" s="76">
+        <f>M5</f>
         <v>0.47249999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" s="49" t="s">
         <v>37</v>
       </c>
@@ -13679,20 +13766,21 @@
       <c r="I6" s="32"/>
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
-      <c r="L6" s="74">
+      <c r="L6" s="81"/>
+      <c r="M6" s="74">
         <f t="shared" si="0"/>
         <v>0.44</v>
       </c>
-      <c r="M6" s="76">
-        <f>L6</f>
+      <c r="N6" s="76">
+        <f>M6</f>
         <v>0.44</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="111">
+      <c r="B7" s="110">
         <f>'Bruil et al. (2025)'!J8-'Bruil et al. (2025)'!J9</f>
         <v>119991</v>
       </c>
@@ -13712,14 +13800,14 @@
         <f>'Bruil et al. (2025)'!C14</f>
         <v>0.12</v>
       </c>
-      <c r="G7" s="109">
+      <c r="G7" s="108">
         <v>0.13</v>
       </c>
       <c r="H7" s="30">
         <f>WID!N23</f>
         <v>5.6364273526328335E-2</v>
       </c>
-      <c r="I7" s="113">
+      <c r="I7" s="112">
         <f>(D7/G7)*(1+H7)^9/1000000</f>
         <v>2.8497031823380623</v>
       </c>
@@ -13731,24 +13819,28 @@
         <f>IF(J$13&lt;=I7, 1, (I7/J$13)^(1/(J7-1)))</f>
         <v>1</v>
       </c>
-      <c r="L7" s="74">
+      <c r="L7" s="63">
+        <f>IF(J$13&lt;=I7, 1, (I7/J$13)^(J7/(J7-1)))*B7</f>
+        <v>119991</v>
+      </c>
+      <c r="M7" s="74">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
-      <c r="M7" s="76">
+      <c r="N7" s="76">
         <f>E7+MAX(0,J$14/G7-F7)*K7</f>
         <v>0.38076923076923075</v>
       </c>
-      <c r="N7" s="99">
-        <f>(M7-L7)*C7*B7*(1+H7)^9/1000000</f>
+      <c r="O7" s="99">
+        <f>(N7-M7)*C7*B7*(1+H7)^9/1000000</f>
         <v>8612.0059524430799</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="111">
+      <c r="B8" s="110">
         <f>'Bruil et al. (2025)'!J9-'Bruil et al. (2025)'!J10</f>
         <v>11999</v>
       </c>
@@ -13768,14 +13860,14 @@
         <f>'Bruil et al. (2025)'!C15</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G8" s="109">
+      <c r="G8" s="108">
         <v>0.12</v>
       </c>
       <c r="H8" s="30">
         <f>WID!N22</f>
         <v>4.3943767809603962E-2</v>
       </c>
-      <c r="I8" s="113">
+      <c r="I8" s="112">
         <f>(D8/G8)*(1+H8)^9/1000000</f>
         <v>12.564966735510884</v>
       </c>
@@ -13787,24 +13879,28 @@
         <f>IF(J$13&lt;=I8, 1, (I8/J$13)^(1/(J8-1)))</f>
         <v>1</v>
       </c>
-      <c r="L8" s="74">
+      <c r="L8" s="63">
+        <f t="shared" ref="L8:L10" si="1">IF(J$13&lt;=I8, 1, (I8/J$13)^(J8/(J8-1)))*B8</f>
+        <v>11999</v>
+      </c>
+      <c r="M8" s="74">
         <f t="shared" si="0"/>
         <v>0.215</v>
       </c>
-      <c r="M8" s="76">
+      <c r="N8" s="76">
         <f>E8+MAX(0,J$14/G8-F8)*K8</f>
         <v>0.39500000000000002</v>
       </c>
-      <c r="N8" s="99">
-        <f>(M8-L8)*C8*B8*(1+H8)^9/1000000</f>
+      <c r="O8" s="99">
+        <f>(N8-M8)*C8*B8*(1+H8)^9/1000000</f>
         <v>5661.7993230749571</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="111">
+      <c r="B9" s="110">
         <f>'Bruil et al. (2025)'!J10-'Bruil et al. (2025)'!J12</f>
         <v>1320</v>
       </c>
@@ -13824,14 +13920,14 @@
         <f>'Bruil et al. (2025)'!C16*0.9 + 'Bruil et al. (2025)'!C17*0.1</f>
         <v>4.3000000000000003E-2</v>
       </c>
-      <c r="G9" s="109">
+      <c r="G9" s="108">
         <v>0.09</v>
       </c>
       <c r="H9" s="30">
         <f>AVERAGE(WID!N20:N21)</f>
         <v>4.056457071269981E-2</v>
       </c>
-      <c r="I9" s="113">
+      <c r="I9" s="112">
         <f>(D9/G9)*(1+H9)^9/1000000</f>
         <v>69.483328167820872</v>
       </c>
@@ -13843,28 +13939,32 @@
         <f>IF(J$13&lt;=I9, 1, (I9/J$13)^(1/(J9-1)))</f>
         <v>1</v>
       </c>
-      <c r="L9" s="74">
+      <c r="L9" s="63">
+        <f t="shared" si="1"/>
+        <v>1320</v>
+      </c>
+      <c r="M9" s="74">
         <f t="shared" si="0"/>
         <v>0.1895</v>
       </c>
-      <c r="M9" s="76">
+      <c r="N9" s="76">
         <f>E9+MAX(0,J$14/G9-F9)*K9</f>
         <v>0.47983333333333333</v>
       </c>
-      <c r="N9" s="99">
-        <f>(M9-L9)*C9*B9*(1+H9)^9/1000000</f>
+      <c r="O9" s="99">
+        <f>(N9-M9)*C9*B9*(1+H9)^9/1000000</f>
         <v>5401.1855549800202</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="111">
+      <c r="B10" s="110">
         <f>'Bruil et al. (2025)'!J12</f>
         <v>14</v>
       </c>
-      <c r="C10" s="112">
+      <c r="C10" s="111">
         <f>'Bruil et al. (2025)'!L12</f>
         <v>111562388</v>
       </c>
@@ -13880,14 +13980,14 @@
         <f>'Bruil et al. (2025)'!C18</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G10" s="137">
+      <c r="G10" s="136">
         <v>0.06</v>
       </c>
       <c r="H10" s="30">
         <f>WID!N20</f>
         <v>3.4737620496357202E-2</v>
       </c>
-      <c r="I10" s="113">
+      <c r="I10" s="112">
         <f>(D10/G10)*(1+H10)^9/1000000</f>
         <v>2034.2728796935851</v>
       </c>
@@ -13899,32 +13999,40 @@
         <f>IF(J$13&lt;=I10, 1, (I10/J$13)^(1/(J10-1)))</f>
         <v>1</v>
       </c>
-      <c r="L10" s="74">
+      <c r="L10" s="63">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="M10" s="74">
         <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
-      <c r="M10" s="76">
+      <c r="N10" s="76">
         <f>E10+MAX(0,J$14/G10-F10)*K10</f>
         <v>0.65500000000000003</v>
       </c>
-      <c r="N10" s="99">
-        <f>(M10-L10)*C10*B10*(1+H10)^9/1000000</f>
+      <c r="O10" s="99">
+        <f>(N10-M10)*C10*B10*(1+H10)^9/1000000</f>
         <v>1051.2915885636514</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" s="49"/>
       <c r="F11" s="45"/>
-      <c r="G11" s="138">
+      <c r="G11" s="137">
         <f>C10*(1+H10)^9/('Billionnaires List'!D7*1000000000/'Billionnaires List'!C7)</f>
         <v>4.0075150220991611E-2</v>
       </c>
-      <c r="N11" s="65">
-        <f>SUM(N7:N10)</f>
+      <c r="L11" s="63">
+        <f>SUM(L7:L10)</f>
+        <v>133324</v>
+      </c>
+      <c r="O11" s="65">
+        <f>SUM(O7:O10)</f>
         <v>20726.282419061707</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="B12" s="8" t="s">
         <v>129</v>
       </c>
@@ -13932,7 +14040,7 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="139" t="s">
+      <c r="G12" s="138" t="s">
         <v>230</v>
       </c>
       <c r="I12" s="145" t="s">
@@ -13940,7 +14048,7 @@
       </c>
       <c r="J12" s="145"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="F13" s="45"/>
       <c r="I13" s="49" t="s">
         <v>73</v>
@@ -13949,7 +14057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="C14" s="42"/>
       <c r="D14" s="42"/>
       <c r="E14" s="42"/>
@@ -13961,13 +14069,13 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="45"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
@@ -13975,7 +14083,7 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="I2:O2"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="G2:H2"/>
@@ -13990,19 +14098,20 @@
   <sheetPr codeName="Feuil4">
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A2:N16"/>
+  <dimension ref="A2:O16"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="11.21875" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="124"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" s="39"/>
       <c r="B2" s="143" t="s">
         <v>183</v>
@@ -14023,18 +14132,19 @@
       <c r="L2" s="144"/>
       <c r="M2" s="144"/>
       <c r="N2" s="144"/>
-    </row>
-    <row r="3" spans="1:14" ht="48">
+      <c r="O2" s="144"/>
+    </row>
+    <row r="3" spans="1:15" ht="48">
       <c r="A3" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="110" t="s">
+      <c r="B3" s="56" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="D3" s="110" t="s">
+      <c r="D3" s="109" t="s">
         <v>224</v>
       </c>
       <c r="E3" s="53" t="s">
@@ -14058,17 +14168,20 @@
       <c r="K3" s="50" t="s">
         <v>196</v>
       </c>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="148" t="s">
+        <v>273</v>
+      </c>
+      <c r="M3" s="56" t="s">
         <v>181</v>
       </c>
-      <c r="M3" s="50" t="s">
+      <c r="N3" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="N3" s="56" t="s">
+      <c r="O3" s="56" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="49" t="s">
         <v>66</v>
       </c>
@@ -14084,16 +14197,17 @@
       <c r="I4" s="32"/>
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
-      <c r="L4" s="73">
-        <f t="shared" ref="L4:L10" si="0">E4</f>
+      <c r="L4" s="81"/>
+      <c r="M4" s="73">
+        <f t="shared" ref="M4:M10" si="0">E4</f>
         <v>0.47672649500000003</v>
       </c>
-      <c r="M4" s="72">
-        <f>L4</f>
+      <c r="N4" s="72">
+        <f>M4</f>
         <v>0.47672649500000003</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" s="49" t="s">
         <v>67</v>
       </c>
@@ -14109,16 +14223,17 @@
       <c r="I5" s="32"/>
       <c r="J5" s="32"/>
       <c r="K5" s="32"/>
-      <c r="L5" s="73">
+      <c r="L5" s="81"/>
+      <c r="M5" s="73">
         <f t="shared" si="0"/>
         <v>0.4674134875</v>
       </c>
-      <c r="M5" s="72">
-        <f>L5</f>
+      <c r="N5" s="72">
+        <f>M5</f>
         <v>0.4674134875</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" s="49" t="s">
         <v>37</v>
       </c>
@@ -14134,16 +14249,17 @@
       <c r="I6" s="32"/>
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
-      <c r="L6" s="73">
+      <c r="L6" s="81"/>
+      <c r="M6" s="73">
         <f t="shared" si="0"/>
         <v>0.46690173999999995</v>
       </c>
-      <c r="M6" s="72">
-        <f>L6</f>
+      <c r="N6" s="72">
+        <f>M6</f>
         <v>0.46690173999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" s="49" t="s">
         <v>38</v>
       </c>
@@ -14167,14 +14283,14 @@
         <f>'Palomo et al. (2025)'!F13 + 'Palomo et al. (2025)'!H13</f>
         <v>9.5415599999999989E-2</v>
       </c>
-      <c r="G7" s="109">
+      <c r="G7" s="108">
         <v>0.13</v>
       </c>
       <c r="H7" s="30">
         <f>WID!N8</f>
         <v>0.13309046810491298</v>
       </c>
-      <c r="I7" s="113">
+      <c r="I7" s="112">
         <f>(D7/G7)*(1+H7)^6/1000000</f>
         <v>1.5129378594561054</v>
       </c>
@@ -14186,20 +14302,24 @@
         <f>IF(J$13&lt;=I7, 1, (I7/J$13)^(1/(J7-1)))</f>
         <v>1</v>
       </c>
-      <c r="L7" s="73">
+      <c r="L7" s="63">
+        <f>IF(J$13&lt;=I7, 1, (I7/J$13)^(J7/(J7-1)))*B7</f>
+        <v>1342683</v>
+      </c>
+      <c r="M7" s="73">
         <f t="shared" si="0"/>
         <v>0.30034454999999999</v>
       </c>
-      <c r="M7" s="72">
+      <c r="N7" s="72">
         <f>E7+MAX(0,J$14/G7-F7)*K7</f>
         <v>0.43569818076923073</v>
       </c>
-      <c r="N7" s="65">
-        <f>(M7-L7)*C7*B7*(1+H7)^6/1000000</f>
+      <c r="O7" s="65">
+        <f>(N7-M7)*C7*B7*(1+H7)^6/1000000</f>
         <v>57918.95864971936</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" s="49" t="s">
         <v>39</v>
       </c>
@@ -14223,14 +14343,14 @@
         <f>'Palomo et al. (2025)'!F14 + 'Palomo et al. (2025)'!H14</f>
         <v>4.8548420000000009E-2</v>
       </c>
-      <c r="G8" s="109">
+      <c r="G8" s="108">
         <v>0.12</v>
       </c>
       <c r="H8" s="30">
         <f>WID!N7</f>
         <v>7.4538792356618311E-2</v>
       </c>
-      <c r="I8" s="113">
+      <c r="I8" s="112">
         <f t="shared" ref="I8:I9" si="1">(D8/G8)*(1+H8)^6/1000000</f>
         <v>4.5272593352047874</v>
       </c>
@@ -14242,20 +14362,24 @@
         <f>IF(J$13&lt;=I8, 1, (I8/J$13)^(1/(J8-1)))</f>
         <v>1</v>
       </c>
-      <c r="L8" s="73">
+      <c r="L8" s="63">
+        <f t="shared" ref="L8:L10" si="2">IF(J$13&lt;=I8, 1, (I8/J$13)^(J8/(J8-1)))*B8</f>
+        <v>134265</v>
+      </c>
+      <c r="M8" s="73">
         <f t="shared" si="0"/>
         <v>0.22436049</v>
       </c>
-      <c r="M8" s="72">
+      <c r="N8" s="72">
         <f>E8+MAX(0,J$14/G8-F8)*K8</f>
         <v>0.42581206999999999</v>
       </c>
-      <c r="N8" s="65">
-        <f t="shared" ref="N8:N10" si="2">(M8-L8)*C8*B8*(1+H8)^6/1000000</f>
+      <c r="O8" s="65">
+        <f t="shared" ref="O8:O10" si="3">(N8-M8)*C8*B8*(1+H8)^6/1000000</f>
         <v>26300.104114851849</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" s="49" t="s">
         <v>84</v>
       </c>
@@ -14279,14 +14403,14 @@
         <f>'Palomo et al. (2025)'!F15 + 'Palomo et al. (2025)'!H15</f>
         <v>3.3692159999999985E-2</v>
       </c>
-      <c r="G9" s="109">
+      <c r="G9" s="108">
         <v>0.09</v>
       </c>
       <c r="H9" s="30">
         <f>AVERAGE(WID!N5:N6)</f>
         <v>5.3320582840966746E-2</v>
       </c>
-      <c r="I9" s="113">
+      <c r="I9" s="112">
         <f t="shared" si="1"/>
         <v>26.372679417922576</v>
       </c>
@@ -14298,20 +14422,24 @@
         <f>IF(J$13&lt;=I9, 1, (I9/J$13)^(1/(J9-1)))</f>
         <v>1</v>
       </c>
-      <c r="L9" s="73">
+      <c r="L9" s="63">
+        <f t="shared" si="2"/>
+        <v>14770</v>
+      </c>
+      <c r="M9" s="73">
         <f t="shared" si="0"/>
         <v>0.21458076000000001</v>
       </c>
-      <c r="M9" s="72">
+      <c r="N9" s="72">
         <f>E9+MAX(0,J$14/G9-F9)*K9</f>
         <v>0.51422193333333333</v>
       </c>
-      <c r="N9" s="65">
-        <f t="shared" si="2"/>
+      <c r="O9" s="65">
+        <f t="shared" si="3"/>
         <v>27187.653587986977</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" s="49" t="s">
         <v>69</v>
       </c>
@@ -14319,7 +14447,7 @@
         <f>'Palomo et al. (2025)'!L12</f>
         <v>152</v>
       </c>
-      <c r="C10" s="114">
+      <c r="C10" s="113">
         <f>'Palomo et al. (2025)'!P12</f>
         <v>121989804.46650124</v>
       </c>
@@ -14335,14 +14463,14 @@
         <f>'Palomo et al. (2025)'!F16 + 'Palomo et al. (2025)'!H16</f>
         <v>2.0460600000000009E-2</v>
       </c>
-      <c r="G10" s="137">
+      <c r="G10" s="136">
         <v>0.06</v>
       </c>
       <c r="H10" s="30">
         <f>WID!N5</f>
         <v>5.3809595206012917E-2</v>
       </c>
-      <c r="I10" s="113">
+      <c r="I10" s="112">
         <f>(D10/G10)*(1+H10)^6/1000000</f>
         <v>1131.0541200678551</v>
       </c>
@@ -14354,32 +14482,40 @@
         <f>IF(J$13&lt;=I10, 1, (I10/J$13)^(1/(J10-1)))</f>
         <v>1</v>
       </c>
-      <c r="L10" s="73">
+      <c r="L10" s="63">
+        <f t="shared" si="2"/>
+        <v>152</v>
+      </c>
+      <c r="M10" s="73">
         <f t="shared" si="0"/>
         <v>0.19708729</v>
       </c>
-      <c r="M10" s="72">
+      <c r="N10" s="72">
         <f>E10+MAX(0,J$14/G10-F10)*K10</f>
         <v>0.67662668999999998</v>
       </c>
-      <c r="N10" s="65">
-        <f t="shared" si="2"/>
+      <c r="O10" s="65">
+        <f t="shared" si="3"/>
         <v>12177.673066567615</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" s="49"/>
       <c r="F11" s="45"/>
-      <c r="G11" s="138">
+      <c r="G11" s="137">
         <f>C10*(1+H10)^6/('Billionnaires List'!D6*1000000000/'Billionnaires List'!C6)</f>
         <v>4.3635853650525774E-2</v>
       </c>
-      <c r="N11" s="65">
-        <f>SUM(N7:N10)</f>
+      <c r="L11" s="63">
+        <f>SUM(L7:L10)</f>
+        <v>1491870</v>
+      </c>
+      <c r="O11" s="65">
+        <f>SUM(O7:O10)</f>
         <v>123584.3894191258</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="B12" s="8" t="s">
         <v>126</v>
       </c>
@@ -14387,7 +14523,7 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="139" t="s">
+      <c r="G12" s="138" t="s">
         <v>231</v>
       </c>
       <c r="I12" s="145" t="s">
@@ -14395,7 +14531,7 @@
       </c>
       <c r="J12" s="145"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="F13" s="45"/>
       <c r="I13" s="49" t="s">
         <v>73</v>
@@ -14404,8 +14540,9 @@
         <v>1</v>
       </c>
       <c r="K13" s="42"/>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="L13" s="42"/>
+    </row>
+    <row r="14" spans="1:15">
       <c r="C14" s="42"/>
       <c r="D14" s="42"/>
       <c r="E14" s="42"/>
@@ -14417,15 +14554,17 @@
         <v>0.03</v>
       </c>
       <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="45"/>
       <c r="K15" s="15"/>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="L15" s="15"/>
+    </row>
+    <row r="16" spans="1:15">
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
@@ -14433,7 +14572,7 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="I2:O2"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="G2:H2"/>
@@ -14448,18 +14587,19 @@
   <sheetPr>
     <tabColor rgb="FF800080"/>
   </sheetPr>
-  <dimension ref="A2:N20"/>
+  <dimension ref="A2:O20"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="124"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" s="39"/>
       <c r="B2" s="143" t="s">
         <v>189</v>
@@ -14480,18 +14620,19 @@
       <c r="L2" s="144"/>
       <c r="M2" s="144"/>
       <c r="N2" s="144"/>
-    </row>
-    <row r="3" spans="1:14" ht="48">
+      <c r="O2" s="144"/>
+    </row>
+    <row r="3" spans="1:15" ht="48">
       <c r="A3" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="110" t="s">
+      <c r="B3" s="56" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" s="109" t="s">
         <v>197</v>
       </c>
-      <c r="D3" s="110" t="s">
+      <c r="D3" s="109" t="s">
         <v>192</v>
       </c>
       <c r="E3" s="53" t="s">
@@ -14515,17 +14656,20 @@
       <c r="K3" s="50" t="s">
         <v>196</v>
       </c>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="148" t="s">
+        <v>273</v>
+      </c>
+      <c r="M3" s="56" t="s">
         <v>181</v>
       </c>
-      <c r="M3" s="56" t="s">
+      <c r="N3" s="56" t="s">
         <v>180</v>
       </c>
-      <c r="N3" s="56" t="s">
+      <c r="O3" s="56" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="49" t="s">
         <v>66</v>
       </c>
@@ -14541,16 +14685,17 @@
       <c r="I4" s="32"/>
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
-      <c r="L4" s="97">
-        <f t="shared" ref="L4:L10" si="0">E4</f>
+      <c r="L4" s="81"/>
+      <c r="M4" s="97">
+        <f t="shared" ref="M4:M10" si="0">E4</f>
         <v>0.42</v>
       </c>
-      <c r="M4" s="96">
-        <f>L4</f>
+      <c r="N4" s="96">
+        <f>M4</f>
         <v>0.42</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" s="49" t="s">
         <v>67</v>
       </c>
@@ -14566,16 +14711,17 @@
       <c r="I5" s="32"/>
       <c r="J5" s="32"/>
       <c r="K5" s="32"/>
-      <c r="L5" s="97">
+      <c r="L5" s="81"/>
+      <c r="M5" s="97">
         <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
-      <c r="M5" s="96">
-        <f>L5</f>
+      <c r="N5" s="96">
+        <f>M5</f>
         <v>0.46</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" s="49" t="s">
         <v>37</v>
       </c>
@@ -14591,16 +14737,17 @@
       <c r="I6" s="32"/>
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
-      <c r="L6" s="97">
+      <c r="L6" s="81"/>
+      <c r="M6" s="97">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="M6" s="96">
-        <f>L6</f>
+      <c r="N6" s="96">
+        <f>M6</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" s="49" t="s">
         <v>38</v>
       </c>
@@ -14624,14 +14771,14 @@
         <f>'Guzzardi et al. (2024)'!D10</f>
         <v>0.25</v>
       </c>
-      <c r="G7" s="109">
+      <c r="G7" s="108">
         <v>0.13</v>
       </c>
       <c r="H7" s="30">
         <f>WID!N18</f>
         <v>4.3673219493195026E-2</v>
       </c>
-      <c r="I7" s="113">
+      <c r="I7" s="112">
         <f>(D7/G7)*(1+H7)^9/1000000</f>
         <v>1.6696099408986425</v>
       </c>
@@ -14640,23 +14787,27 @@
         <v>1.4373127783966266</v>
       </c>
       <c r="K7" s="94">
-        <f>IF(L$13&lt;=I7, 1, (I7/L$13)^(1/(J7-1)))</f>
+        <f>IF(J$13&lt;=I7, 1, (I7/J$13)^(1/(J7-1)))</f>
         <v>1</v>
       </c>
-      <c r="L7" s="97">
+      <c r="L7" s="63">
+        <f>IF(J$13&lt;=I7, 1, (I7/J$13)^(J7/(J7-1)))*B7</f>
+        <v>456295</v>
+      </c>
+      <c r="M7" s="97">
         <f t="shared" si="0"/>
         <v>0.43</v>
       </c>
-      <c r="M7" s="96">
-        <f>E7+MAX(0,L$14/G7-F7)*K7</f>
+      <c r="N7" s="96">
+        <f>E7+MAX(0,J$14/G7-F7)*K7</f>
         <v>0.43</v>
       </c>
-      <c r="N7" s="65">
-        <f>(M7-L7)*C7*B7*(1+H7)^9/1000000</f>
+      <c r="O7" s="65">
+        <f>(N7-M7)*C7*B7*(1+H7)^9/1000000</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" s="49" t="s">
         <v>39</v>
       </c>
@@ -14680,14 +14831,14 @@
         <f>'Guzzardi et al. (2024)'!D11</f>
         <v>0.15</v>
       </c>
-      <c r="G8" s="109">
+      <c r="G8" s="108">
         <v>0.12</v>
       </c>
       <c r="H8" s="30">
         <f>WID!N17</f>
         <v>6.5618761329873765E-2</v>
       </c>
-      <c r="I8" s="113">
+      <c r="I8" s="112">
         <f>(D8/G8)*(1+H8)^9/1000000</f>
         <v>7.4939073466760009</v>
       </c>
@@ -14696,23 +14847,27 @@
         <v>1.2178724747155847</v>
       </c>
       <c r="K8" s="94">
-        <f>IF(L$13&lt;=I8, 1, (I8/L$13)^(1/(J8-1)))</f>
+        <f>IF(J$13&lt;=I8, 1, (I8/J$13)^(1/(J8-1)))</f>
         <v>1</v>
       </c>
-      <c r="L8" s="97">
+      <c r="L8" s="63">
+        <f t="shared" ref="L8:L10" si="1">IF(J$13&lt;=I8, 1, (I8/J$13)^(J8/(J8-1)))*B8</f>
+        <v>50699</v>
+      </c>
+      <c r="M8" s="97">
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
-      <c r="M8" s="96">
-        <f>E8+MAX(0,L$14/G8-F8)*K8</f>
+      <c r="N8" s="96">
+        <f>E8+MAX(0,J$14/G8-F8)*K8</f>
         <v>0.45999999999999996</v>
       </c>
-      <c r="N8" s="65">
-        <f>(M8-L8)*C8*B8*(1+H8)^9/1000000</f>
+      <c r="O8" s="65">
+        <f>(N8-M8)*C8*B8*(1+H8)^9/1000000</f>
         <v>5552.5282091484514</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" s="49" t="s">
         <v>84</v>
       </c>
@@ -14736,14 +14891,14 @@
         <f>AVERAGE('Guzzardi et al. (2024)'!C11:C12)*('Guzzardi et al. (2024)'!D11/'Guzzardi et al. (2024)'!C11)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="G9" s="109">
+      <c r="G9" s="108">
         <v>0.09</v>
       </c>
       <c r="H9" s="30">
         <f>AVERAGE(WID!N15:N16)</f>
         <v>8.1284523033389955E-2</v>
       </c>
-      <c r="I9" s="113">
+      <c r="I9" s="112">
         <f>(D9/G9)*(1+H9)^9/1000000</f>
         <v>33.892192798415643</v>
       </c>
@@ -14752,23 +14907,27 @@
         <v>2.5848609363138757</v>
       </c>
       <c r="K9" s="94">
-        <f>IF(L$13&lt;=I9, 1, (I9/L$13)^(1/(J9-1)))</f>
+        <f>IF(J$13&lt;=I9, 1, (I9/J$13)^(1/(J9-1)))</f>
         <v>1</v>
       </c>
-      <c r="L9" s="97">
+      <c r="L9" s="63">
+        <f t="shared" si="1"/>
+        <v>5069.8999999999996</v>
+      </c>
+      <c r="M9" s="97">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
-      <c r="M9" s="96">
-        <f>E9+MAX(0,L$14/G9-F9)*K9</f>
+      <c r="N9" s="96">
+        <f>E9+MAX(0,J$14/G9-F9)*K9</f>
         <v>0.49083333333333334</v>
       </c>
-      <c r="N9" s="65">
-        <f>(M9-L9)*C9*B9*(1+H9)^9/1000000</f>
+      <c r="O9" s="65">
+        <f>(N9-M9)*C9*B9*(1+H9)^9/1000000</f>
         <v>8827.6149641791053</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" s="49" t="s">
         <v>69</v>
       </c>
@@ -14792,14 +14951,14 @@
         <f>'Guzzardi et al. (2024)'!C12*('Guzzardi et al. (2024)'!D11/'Guzzardi et al. (2024)'!C11)</f>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G10" s="137">
+      <c r="G10" s="136">
         <v>0.06</v>
       </c>
       <c r="H10" s="30">
         <f>WID!N15</f>
         <v>8.8542974272436403E-2</v>
       </c>
-      <c r="I10" s="113">
+      <c r="I10" s="112">
         <f>(D10/G10)*(1+H10)^9/1000000</f>
         <v>2563.1539210969795</v>
       </c>
@@ -14808,35 +14967,43 @@
         <v>3.5308579785505363</v>
       </c>
       <c r="K10" s="94">
-        <f>IF(L$13&lt;=I10, 1, (I10/L$13)^(1/(J10-1)))</f>
+        <f>IF(J$13&lt;=I10, 1, (I10/J$13)^(1/(J10-1)))</f>
         <v>1</v>
       </c>
-      <c r="L10" s="97">
+      <c r="L10" s="63">
+        <f t="shared" si="1"/>
+        <v>50.698999999999998</v>
+      </c>
+      <c r="M10" s="97">
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
-      <c r="M10" s="96">
-        <f>E10+MAX(0,L$14/G10-F10)*K10</f>
+      <c r="N10" s="96">
+        <f>E10+MAX(0,J$14/G10-F10)*K10</f>
         <v>0.60499999999999998</v>
       </c>
-      <c r="N10" s="65">
-        <f>(M10-L10)*C10*B10*(1+H10)^9/1000000</f>
+      <c r="O10" s="65">
+        <f>(N10-M10)*C10*B10*(1+H10)^9/1000000</f>
         <v>11700.232988769027</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" s="49"/>
       <c r="F11" s="45"/>
-      <c r="G11" s="138">
+      <c r="G11" s="137">
         <f>C10*(1+H10)^9/('Billionnaires List'!E5*1000000000/'Billionnaires List'!C5)</f>
         <v>0.12517340663675089</v>
       </c>
-      <c r="N11" s="100">
-        <f>SUM(N7:N10)</f>
+      <c r="L11" s="63">
+        <f>SUM(L7:L10)</f>
+        <v>512114.59900000005</v>
+      </c>
+      <c r="O11" s="100">
+        <f>SUM(O7:O10)</f>
         <v>26080.376162096582</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="B12" s="8" t="s">
         <v>176</v>
       </c>
@@ -14844,45 +15011,45 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="139" t="s">
+      <c r="G12" s="138" t="s">
         <v>229</v>
       </c>
-      <c r="K12" s="145" t="s">
+      <c r="I12" s="145" t="s">
         <v>77</v>
       </c>
-      <c r="L12" s="145"/>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="J12" s="145"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="B13" t="s">
         <v>190</v>
       </c>
       <c r="F13" s="45"/>
-      <c r="K13" s="49" t="s">
+      <c r="I13" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="L13" s="5">
+      <c r="J13" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="B14" t="s">
         <v>199</v>
       </c>
       <c r="F14" s="45"/>
-      <c r="K14" s="49" t="s">
+      <c r="I14" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="L14" s="15">
+      <c r="J14" s="15">
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="B15" t="s">
         <v>177</v>
       </c>
       <c r="F15" s="45"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="B16" t="s">
         <v>198</v>
       </c>
@@ -14911,9 +15078,9 @@
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="I12:J12"/>
     <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="I2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14925,7 +15092,7 @@
   <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -15313,7 +15480,7 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="B2:Q52"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
@@ -17107,7 +17274,7 @@
   <dimension ref="B2:L26"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -17558,13 +17725,13 @@
       <c r="B15" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="116">
+      <c r="C15" s="115">
         <v>1950271</v>
       </c>
-      <c r="D15" s="117">
+      <c r="D15" s="116">
         <v>936385</v>
       </c>
-      <c r="E15" s="115">
+      <c r="E15" s="114">
         <v>539000</v>
       </c>
       <c r="F15" s="79">
@@ -17593,13 +17760,13 @@
       <c r="B16" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="116">
+      <c r="C16" s="115">
         <v>195016</v>
       </c>
-      <c r="D16" s="117">
+      <c r="D16" s="116">
         <v>4526004</v>
       </c>
-      <c r="E16" s="115">
+      <c r="E16" s="114">
         <v>2430000</v>
       </c>
       <c r="F16" s="79">
@@ -17628,13 +17795,13 @@
       <c r="B17" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="116">
+      <c r="C17" s="115">
         <v>21163</v>
       </c>
-      <c r="D17" s="117">
+      <c r="D17" s="116">
         <v>31593939</v>
       </c>
-      <c r="E17" s="115">
+      <c r="E17" s="114">
         <v>12800000</v>
       </c>
       <c r="F17" s="79">
@@ -17666,7 +17833,7 @@
       <c r="C18" s="86">
         <v>515</v>
       </c>
-      <c r="D18" s="102">
+      <c r="D18" s="87">
         <v>207996848</v>
       </c>
       <c r="E18" s="101"/>

</xml_diff>